<commit_message>
Added Sync D-FF to write input of memory ICs
Needed to rework microcode....
should hopefully prevent any glitches on the ram/stack write line causing accidental writes.
</commit_message>
<xml_diff>
--- a/ROMGeneration/MicroCodeRoms.xlsx
+++ b/ROMGeneration/MicroCodeRoms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\ROMGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3909A4-22B2-4811-B0E5-3C9E27644D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF978F9-B30A-473D-9854-D90FF955EEC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
   </bookViews>
   <sheets>
     <sheet name="ControlRoms" sheetId="1" r:id="rId1"/>
@@ -909,9 +909,6 @@
     <t>Stack_DEC_EN</t>
   </si>
   <si>
-    <t>Stack_INC_EN</t>
-  </si>
-  <si>
     <t>ROM 0</t>
   </si>
   <si>
@@ -966,19 +963,10 @@
     <t>CO_In[0..7]-&gt;DBus</t>
   </si>
   <si>
-    <t>Stack_LatchSafeD_EN</t>
-  </si>
-  <si>
     <t>RAM_LatchSafeDA_EN</t>
   </si>
   <si>
     <t>RAM_RAsync_LatchSafeA</t>
-  </si>
-  <si>
-    <t>RAM_WAsync</t>
-  </si>
-  <si>
-    <t>Stack_WAsync</t>
   </si>
   <si>
     <t>Stack_RAsync</t>
@@ -1006,6 +994,18 @@
   </si>
   <si>
     <t>Logic_Comp_OE</t>
+  </si>
+  <si>
+    <t>Stack_INC+LatchSafeD_EN</t>
+  </si>
+  <si>
+    <t>Stack_PresentData</t>
+  </si>
+  <si>
+    <t>Stack_W</t>
+  </si>
+  <si>
+    <t>RAM_W</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1053,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1332,20 +1332,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1403,9 +1394,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1459,9 +1447,44 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1546,7 +1569,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1848,11 +1871,11 @@
   <dimension ref="A1:AR260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
+      <pane ySplit="2" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="11" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="5" customWidth="1"/>
@@ -1931,17 +1954,17 @@
       <c r="AQ1" s="7"/>
       <c r="AR1" s="12"/>
     </row>
-    <row r="2" spans="1:44" s="1" customFormat="1" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="27" t="s">
+    <row r="2" spans="1:44" s="1" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1963,7 +1986,7 @@
         <v>267</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="L2" s="18"/>
       <c r="M2" s="15" t="s">
@@ -2003,7 +2026,7 @@
         <v>285</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="Z2" s="16" t="s">
         <v>281</v>
@@ -2030,40 +2053,40 @@
         <v>289</v>
       </c>
       <c r="AH2" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AI2" s="17"/>
       <c r="AJ2" s="18"/>
       <c r="AK2" s="15" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="AL2" s="16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AM2" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="AN2" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO2" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="AN2" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="AO2" s="17" t="s">
-        <v>316</v>
-      </c>
       <c r="AP2" s="16" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="AQ2" s="17" t="s">
         <v>291</v>
       </c>
       <c r="AR2" s="18" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="19">
         <v>0</v>
       </c>
@@ -2186,63 +2209,63 @@
       </c>
     </row>
     <row r="4" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="36" t="s">
-        <v>293</v>
-      </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="33" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="36" t="s">
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="33" t="s">
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="33" t="s">
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="33"/>
+      <c r="AF4" s="33"/>
+      <c r="AG4" s="33"/>
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="33"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="35"/>
+      <c r="AL4" s="33"/>
+      <c r="AM4" s="33"/>
+      <c r="AN4" s="33"/>
+      <c r="AO4" s="33"/>
+      <c r="AP4" s="33"/>
+      <c r="AQ4" s="33"/>
+      <c r="AR4" s="34"/>
     </row>
     <row r="5" spans="1:44" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>263</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2376,7 +2399,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -2508,7 +2531,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -2640,7 +2663,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -2772,7 +2795,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2904,7 +2927,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
@@ -3036,7 +3059,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
@@ -3168,7 +3191,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
@@ -3300,7 +3323,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>270</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3434,7 +3457,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
@@ -3566,7 +3589,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -3698,7 +3721,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>18</v>
       </c>
@@ -3830,7 +3853,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
@@ -3962,7 +3985,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4117,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
@@ -4226,7 +4249,7 @@
       </c>
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="5" t="s">
         <v>22</v>
       </c>
@@ -4358,8 +4381,8 @@
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>294</v>
+      <c r="A21" s="21" t="s">
+        <v>293</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>23</v>
@@ -4492,7 +4515,7 @@
       </c>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>24</v>
       </c>
@@ -4624,7 +4647,7 @@
       </c>
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="5" t="s">
         <v>25</v>
       </c>
@@ -4756,7 +4779,7 @@
       </c>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
@@ -4888,7 +4911,7 @@
       </c>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="5" t="s">
         <v>27</v>
       </c>
@@ -5020,7 +5043,7 @@
       </c>
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5" t="s">
         <v>28</v>
       </c>
@@ -5152,7 +5175,7 @@
       </c>
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
         <v>29</v>
       </c>
@@ -5284,7 +5307,7 @@
       </c>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
@@ -5416,8 +5439,8 @@
       </c>
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>295</v>
+      <c r="A29" s="21" t="s">
+        <v>294</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>31</v>
@@ -5550,7 +5573,7 @@
       </c>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
@@ -5682,7 +5705,7 @@
       </c>
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
@@ -5692,8 +5715,8 @@
       <c r="D31" s="3">
         <v>2</v>
       </c>
-      <c r="E31" s="8">
-        <v>1</v>
+      <c r="E31" s="9">
+        <v>0</v>
       </c>
       <c r="F31" s="9">
         <v>0</v>
@@ -5701,8 +5724,8 @@
       <c r="G31" s="9">
         <v>0</v>
       </c>
-      <c r="H31" s="9">
-        <v>1</v>
+      <c r="H31" s="10">
+        <v>0</v>
       </c>
       <c r="I31" s="9">
         <v>0</v>
@@ -5720,7 +5743,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O31" s="9">
         <v>0</v>
@@ -5798,7 +5821,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="9">
         <v>0</v>
@@ -5814,7 +5837,7 @@
       </c>
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="5" t="s">
         <v>34</v>
       </c>
@@ -5825,7 +5848,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="9">
         <v>0</v>
@@ -5834,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="9">
         <v>0</v>
@@ -5930,13 +5953,13 @@
         <v>0</v>
       </c>
       <c r="AN32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO32" s="9">
         <v>0</v>
       </c>
       <c r="AP32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ32" s="9">
         <v>0</v>
@@ -5946,7 +5969,7 @@
       </c>
     </row>
     <row r="33" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>35</v>
       </c>
@@ -6078,7 +6101,7 @@
       </c>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>36</v>
       </c>
@@ -6210,7 +6233,7 @@
       </c>
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5" t="s">
         <v>37</v>
       </c>
@@ -6342,7 +6365,7 @@
       </c>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="5" t="s">
         <v>38</v>
       </c>
@@ -6474,8 +6497,8 @@
       </c>
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
-        <v>296</v>
+      <c r="A37" s="21" t="s">
+        <v>295</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>39</v>
@@ -6608,7 +6631,7 @@
       </c>
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="5" t="s">
         <v>40</v>
       </c>
@@ -6740,7 +6763,7 @@
       </c>
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="5" t="s">
         <v>41</v>
       </c>
@@ -6872,7 +6895,7 @@
       </c>
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="5" t="s">
         <v>42</v>
       </c>
@@ -7004,7 +7027,7 @@
       </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="5" t="s">
         <v>43</v>
       </c>
@@ -7136,7 +7159,7 @@
       </c>
     </row>
     <row r="42" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="5" t="s">
         <v>44</v>
       </c>
@@ -7268,7 +7291,7 @@
       </c>
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="5" t="s">
         <v>45</v>
       </c>
@@ -7400,7 +7423,7 @@
       </c>
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="5" t="s">
         <v>46</v>
       </c>
@@ -7532,8 +7555,8 @@
       </c>
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A45" s="22" t="s">
-        <v>297</v>
+      <c r="A45" s="21" t="s">
+        <v>296</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>47</v>
@@ -7666,7 +7689,7 @@
       </c>
     </row>
     <row r="46" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="5" t="s">
         <v>48</v>
       </c>
@@ -7798,7 +7821,7 @@
       </c>
     </row>
     <row r="47" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="5" t="s">
         <v>49</v>
       </c>
@@ -7930,7 +7953,7 @@
       </c>
     </row>
     <row r="48" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="5" t="s">
         <v>50</v>
       </c>
@@ -8062,7 +8085,7 @@
       </c>
     </row>
     <row r="49" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A49" s="22"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="5" t="s">
         <v>51</v>
       </c>
@@ -8194,7 +8217,7 @@
       </c>
     </row>
     <row r="50" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="5" t="s">
         <v>52</v>
       </c>
@@ -8326,7 +8349,7 @@
       </c>
     </row>
     <row r="51" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
         <v>53</v>
       </c>
@@ -8458,7 +8481,7 @@
       </c>
     </row>
     <row r="52" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="5" t="s">
         <v>54</v>
       </c>
@@ -8590,8 +8613,8 @@
       </c>
     </row>
     <row r="53" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A53" s="22" t="s">
-        <v>298</v>
+      <c r="A53" s="21" t="s">
+        <v>297</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>55</v>
@@ -8724,7 +8747,7 @@
       </c>
     </row>
     <row r="54" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="5" t="s">
         <v>56</v>
       </c>
@@ -8856,7 +8879,7 @@
       </c>
     </row>
     <row r="55" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>57</v>
       </c>
@@ -8988,7 +9011,7 @@
       </c>
     </row>
     <row r="56" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
         <v>58</v>
       </c>
@@ -9120,7 +9143,7 @@
       </c>
     </row>
     <row r="57" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A57" s="22"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="5" t="s">
         <v>59</v>
       </c>
@@ -9252,7 +9275,7 @@
       </c>
     </row>
     <row r="58" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A58" s="22"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="5" t="s">
         <v>60</v>
       </c>
@@ -9384,7 +9407,7 @@
       </c>
     </row>
     <row r="59" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A59" s="22"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="5" t="s">
         <v>61</v>
       </c>
@@ -9516,7 +9539,7 @@
       </c>
     </row>
     <row r="60" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A60" s="22"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="5" t="s">
         <v>62</v>
       </c>
@@ -9648,8 +9671,8 @@
       </c>
     </row>
     <row r="61" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A61" s="22" t="s">
-        <v>299</v>
+      <c r="A61" s="21" t="s">
+        <v>298</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>63</v>
@@ -9782,7 +9805,7 @@
       </c>
     </row>
     <row r="62" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>64</v>
       </c>
@@ -9914,7 +9937,7 @@
       </c>
     </row>
     <row r="63" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>65</v>
       </c>
@@ -10046,7 +10069,7 @@
       </c>
     </row>
     <row r="64" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A64" s="22"/>
+      <c r="A64" s="21"/>
       <c r="B64" s="5" t="s">
         <v>66</v>
       </c>
@@ -10178,7 +10201,7 @@
       </c>
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A65" s="22"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>67</v>
       </c>
@@ -10310,7 +10333,7 @@
       </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A66" s="22"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>68</v>
       </c>
@@ -10442,7 +10465,7 @@
       </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A67" s="22"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="5" t="s">
         <v>69</v>
       </c>
@@ -10574,7 +10597,7 @@
       </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A68" s="22"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="5" t="s">
         <v>70</v>
       </c>
@@ -10706,8 +10729,8 @@
       </c>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A69" s="22" t="s">
-        <v>300</v>
+      <c r="A69" s="21" t="s">
+        <v>299</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>71</v>
@@ -10840,7 +10863,7 @@
       </c>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A70" s="22"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="5" t="s">
         <v>72</v>
       </c>
@@ -10972,7 +10995,7 @@
       </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A71" s="22"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="5" t="s">
         <v>73</v>
       </c>
@@ -11104,7 +11127,7 @@
       </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A72" s="22"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="5" t="s">
         <v>74</v>
       </c>
@@ -11236,7 +11259,7 @@
       </c>
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A73" s="22"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="5" t="s">
         <v>75</v>
       </c>
@@ -11368,7 +11391,7 @@
       </c>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A74" s="22"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="5" t="s">
         <v>76</v>
       </c>
@@ -11500,7 +11523,7 @@
       </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A75" s="22"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="5" t="s">
         <v>77</v>
       </c>
@@ -11632,7 +11655,7 @@
       </c>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A76" s="22"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="5" t="s">
         <v>78</v>
       </c>
@@ -11764,8 +11787,8 @@
       </c>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A77" s="22" t="s">
-        <v>301</v>
+      <c r="A77" s="21" t="s">
+        <v>300</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>79</v>
@@ -11898,7 +11921,7 @@
       </c>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A78" s="22"/>
+      <c r="A78" s="21"/>
       <c r="B78" s="5" t="s">
         <v>80</v>
       </c>
@@ -12030,7 +12053,7 @@
       </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A79" s="22"/>
+      <c r="A79" s="21"/>
       <c r="B79" s="5" t="s">
         <v>81</v>
       </c>
@@ -12162,7 +12185,7 @@
       </c>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A80" s="22"/>
+      <c r="A80" s="21"/>
       <c r="B80" s="5" t="s">
         <v>82</v>
       </c>
@@ -12294,7 +12317,7 @@
       </c>
     </row>
     <row r="81" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A81" s="22"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="5" t="s">
         <v>83</v>
       </c>
@@ -12426,7 +12449,7 @@
       </c>
     </row>
     <row r="82" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A82" s="22"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="5" t="s">
         <v>84</v>
       </c>
@@ -12558,7 +12581,7 @@
       </c>
     </row>
     <row r="83" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A83" s="22"/>
+      <c r="A83" s="21"/>
       <c r="B83" s="5" t="s">
         <v>85</v>
       </c>
@@ -12690,7 +12713,7 @@
       </c>
     </row>
     <row r="84" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A84" s="22"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="5" t="s">
         <v>86</v>
       </c>
@@ -12822,8 +12845,8 @@
       </c>
     </row>
     <row r="85" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A85" s="22" t="s">
-        <v>321</v>
+      <c r="A85" s="21" t="s">
+        <v>317</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>87</v>
@@ -12956,7 +12979,7 @@
       </c>
     </row>
     <row r="86" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
+      <c r="A86" s="21"/>
       <c r="B86" s="5" t="s">
         <v>88</v>
       </c>
@@ -13088,7 +13111,7 @@
       </c>
     </row>
     <row r="87" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A87" s="22"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="5" t="s">
         <v>89</v>
       </c>
@@ -13220,7 +13243,7 @@
       </c>
     </row>
     <row r="88" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A88" s="22"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="5" t="s">
         <v>90</v>
       </c>
@@ -13352,7 +13375,7 @@
       </c>
     </row>
     <row r="89" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A89" s="22"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="5" t="s">
         <v>91</v>
       </c>
@@ -13484,7 +13507,7 @@
       </c>
     </row>
     <row r="90" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A90" s="22"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="5" t="s">
         <v>92</v>
       </c>
@@ -13616,7 +13639,7 @@
       </c>
     </row>
     <row r="91" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A91" s="22"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="5" t="s">
         <v>93</v>
       </c>
@@ -13748,7 +13771,7 @@
       </c>
     </row>
     <row r="92" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A92" s="22"/>
+      <c r="A92" s="21"/>
       <c r="B92" s="5" t="s">
         <v>94</v>
       </c>
@@ -13880,8 +13903,8 @@
       </c>
     </row>
     <row r="93" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A93" s="22" t="s">
-        <v>322</v>
+      <c r="A93" s="21" t="s">
+        <v>318</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>95</v>
@@ -14014,7 +14037,7 @@
       </c>
     </row>
     <row r="94" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A94" s="22"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="5" t="s">
         <v>96</v>
       </c>
@@ -14024,7 +14047,7 @@
       <c r="D94" s="3">
         <v>1</v>
       </c>
-      <c r="E94" s="8">
+      <c r="E94" s="9">
         <v>0</v>
       </c>
       <c r="F94" s="9">
@@ -14033,7 +14056,7 @@
       <c r="G94" s="9">
         <v>0</v>
       </c>
-      <c r="H94" s="9">
+      <c r="H94" s="10">
         <v>0</v>
       </c>
       <c r="I94" s="9">
@@ -14146,7 +14169,7 @@
       </c>
     </row>
     <row r="95" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A95" s="22"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="5" t="s">
         <v>97</v>
       </c>
@@ -14156,8 +14179,8 @@
       <c r="D95" s="3">
         <v>2</v>
       </c>
-      <c r="E95" s="8">
-        <v>1</v>
+      <c r="E95" s="9">
+        <v>0</v>
       </c>
       <c r="F95" s="9">
         <v>0</v>
@@ -14165,8 +14188,8 @@
       <c r="G95" s="9">
         <v>0</v>
       </c>
-      <c r="H95" s="9">
-        <v>1</v>
+      <c r="H95" s="10">
+        <v>0</v>
       </c>
       <c r="I95" s="9">
         <v>0</v>
@@ -14278,7 +14301,7 @@
       </c>
     </row>
     <row r="96" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A96" s="22"/>
+      <c r="A96" s="21"/>
       <c r="B96" s="5" t="s">
         <v>98</v>
       </c>
@@ -14289,7 +14312,7 @@
         <v>3</v>
       </c>
       <c r="E96" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" s="9">
         <v>0</v>
@@ -14298,7 +14321,7 @@
         <v>0</v>
       </c>
       <c r="H96" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" s="9">
         <v>0</v>
@@ -14316,7 +14339,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O96" s="9">
         <v>0</v>
@@ -14373,7 +14396,7 @@
         <v>0</v>
       </c>
       <c r="AG96" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH96" s="9">
         <v>0</v>
@@ -14391,7 +14414,7 @@
         <v>0</v>
       </c>
       <c r="AM96" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN96" s="9">
         <v>0</v>
@@ -14410,7 +14433,7 @@
       </c>
     </row>
     <row r="97" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A97" s="22"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="5" t="s">
         <v>99</v>
       </c>
@@ -14542,7 +14565,7 @@
       </c>
     </row>
     <row r="98" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A98" s="22"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="5" t="s">
         <v>100</v>
       </c>
@@ -14674,7 +14697,7 @@
       </c>
     </row>
     <row r="99" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A99" s="22"/>
+      <c r="A99" s="21"/>
       <c r="B99" s="5" t="s">
         <v>101</v>
       </c>
@@ -14806,7 +14829,7 @@
       </c>
     </row>
     <row r="100" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A100" s="22"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="5" t="s">
         <v>102</v>
       </c>
@@ -14938,8 +14961,8 @@
       </c>
     </row>
     <row r="101" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A101" s="22" t="s">
-        <v>302</v>
+      <c r="A101" s="21" t="s">
+        <v>301</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>103</v>
@@ -15072,7 +15095,7 @@
       </c>
     </row>
     <row r="102" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A102" s="22"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="5" t="s">
         <v>104</v>
       </c>
@@ -15204,7 +15227,7 @@
       </c>
     </row>
     <row r="103" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A103" s="22"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="5" t="s">
         <v>105</v>
       </c>
@@ -15336,7 +15359,7 @@
       </c>
     </row>
     <row r="104" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A104" s="22"/>
+      <c r="A104" s="21"/>
       <c r="B104" s="5" t="s">
         <v>106</v>
       </c>
@@ -15468,7 +15491,7 @@
       </c>
     </row>
     <row r="105" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A105" s="22"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="5" t="s">
         <v>107</v>
       </c>
@@ -15600,7 +15623,7 @@
       </c>
     </row>
     <row r="106" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A106" s="22"/>
+      <c r="A106" s="21"/>
       <c r="B106" s="5" t="s">
         <v>108</v>
       </c>
@@ -15732,7 +15755,7 @@
       </c>
     </row>
     <row r="107" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A107" s="22"/>
+      <c r="A107" s="21"/>
       <c r="B107" s="5" t="s">
         <v>109</v>
       </c>
@@ -15864,7 +15887,7 @@
       </c>
     </row>
     <row r="108" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A108" s="22"/>
+      <c r="A108" s="21"/>
       <c r="B108" s="5" t="s">
         <v>110</v>
       </c>
@@ -15996,8 +16019,8 @@
       </c>
     </row>
     <row r="109" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A109" s="22" t="s">
-        <v>303</v>
+      <c r="A109" s="21" t="s">
+        <v>302</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>111</v>
@@ -16130,7 +16153,7 @@
       </c>
     </row>
     <row r="110" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A110" s="22"/>
+      <c r="A110" s="21"/>
       <c r="B110" s="5" t="s">
         <v>112</v>
       </c>
@@ -16262,7 +16285,7 @@
       </c>
     </row>
     <row r="111" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A111" s="22"/>
+      <c r="A111" s="21"/>
       <c r="B111" s="5" t="s">
         <v>113</v>
       </c>
@@ -16394,7 +16417,7 @@
       </c>
     </row>
     <row r="112" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A112" s="22"/>
+      <c r="A112" s="21"/>
       <c r="B112" s="5" t="s">
         <v>114</v>
       </c>
@@ -16526,7 +16549,7 @@
       </c>
     </row>
     <row r="113" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A113" s="22"/>
+      <c r="A113" s="21"/>
       <c r="B113" s="5" t="s">
         <v>115</v>
       </c>
@@ -16658,7 +16681,7 @@
       </c>
     </row>
     <row r="114" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A114" s="22"/>
+      <c r="A114" s="21"/>
       <c r="B114" s="5" t="s">
         <v>116</v>
       </c>
@@ -16790,7 +16813,7 @@
       </c>
     </row>
     <row r="115" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A115" s="22"/>
+      <c r="A115" s="21"/>
       <c r="B115" s="5" t="s">
         <v>117</v>
       </c>
@@ -16922,7 +16945,7 @@
       </c>
     </row>
     <row r="116" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A116" s="22"/>
+      <c r="A116" s="21"/>
       <c r="B116" s="5" t="s">
         <v>118</v>
       </c>
@@ -17054,8 +17077,8 @@
       </c>
     </row>
     <row r="117" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A117" s="22" t="s">
-        <v>304</v>
+      <c r="A117" s="21" t="s">
+        <v>303</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>119</v>
@@ -17188,7 +17211,7 @@
       </c>
     </row>
     <row r="118" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A118" s="22"/>
+      <c r="A118" s="21"/>
       <c r="B118" s="5" t="s">
         <v>120</v>
       </c>
@@ -17320,7 +17343,7 @@
       </c>
     </row>
     <row r="119" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A119" s="22"/>
+      <c r="A119" s="21"/>
       <c r="B119" s="5" t="s">
         <v>121</v>
       </c>
@@ -17452,7 +17475,7 @@
       </c>
     </row>
     <row r="120" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A120" s="22"/>
+      <c r="A120" s="21"/>
       <c r="B120" s="5" t="s">
         <v>122</v>
       </c>
@@ -17584,7 +17607,7 @@
       </c>
     </row>
     <row r="121" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A121" s="22"/>
+      <c r="A121" s="21"/>
       <c r="B121" s="5" t="s">
         <v>123</v>
       </c>
@@ -17716,7 +17739,7 @@
       </c>
     </row>
     <row r="122" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A122" s="22"/>
+      <c r="A122" s="21"/>
       <c r="B122" s="5" t="s">
         <v>124</v>
       </c>
@@ -17848,7 +17871,7 @@
       </c>
     </row>
     <row r="123" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A123" s="22"/>
+      <c r="A123" s="21"/>
       <c r="B123" s="5" t="s">
         <v>125</v>
       </c>
@@ -17980,7 +18003,7 @@
       </c>
     </row>
     <row r="124" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A124" s="22"/>
+      <c r="A124" s="21"/>
       <c r="B124" s="5" t="s">
         <v>126</v>
       </c>
@@ -18112,8 +18135,8 @@
       </c>
     </row>
     <row r="125" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A125" s="22" t="s">
-        <v>305</v>
+      <c r="A125" s="21" t="s">
+        <v>304</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>127</v>
@@ -18246,7 +18269,7 @@
       </c>
     </row>
     <row r="126" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A126" s="22"/>
+      <c r="A126" s="21"/>
       <c r="B126" s="5" t="s">
         <v>128</v>
       </c>
@@ -18378,7 +18401,7 @@
       </c>
     </row>
     <row r="127" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A127" s="22"/>
+      <c r="A127" s="21"/>
       <c r="B127" s="5" t="s">
         <v>129</v>
       </c>
@@ -18510,7 +18533,7 @@
       </c>
     </row>
     <row r="128" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A128" s="22"/>
+      <c r="A128" s="21"/>
       <c r="B128" s="5" t="s">
         <v>130</v>
       </c>
@@ -18642,7 +18665,7 @@
       </c>
     </row>
     <row r="129" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A129" s="22"/>
+      <c r="A129" s="21"/>
       <c r="B129" s="5" t="s">
         <v>131</v>
       </c>
@@ -18774,7 +18797,7 @@
       </c>
     </row>
     <row r="130" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A130" s="22"/>
+      <c r="A130" s="21"/>
       <c r="B130" s="5" t="s">
         <v>132</v>
       </c>
@@ -18906,7 +18929,7 @@
       </c>
     </row>
     <row r="131" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A131" s="22"/>
+      <c r="A131" s="21"/>
       <c r="B131" s="5" t="s">
         <v>133</v>
       </c>
@@ -19038,7 +19061,7 @@
       </c>
     </row>
     <row r="132" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A132" s="22"/>
+      <c r="A132" s="21"/>
       <c r="B132" s="5" t="s">
         <v>134</v>
       </c>
@@ -19170,8 +19193,8 @@
       </c>
     </row>
     <row r="133" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A133" s="22" t="s">
-        <v>318</v>
+      <c r="A133" s="21" t="s">
+        <v>314</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>135</v>
@@ -19304,7 +19327,7 @@
       </c>
     </row>
     <row r="134" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A134" s="22"/>
+      <c r="A134" s="21"/>
       <c r="B134" s="5" t="s">
         <v>136</v>
       </c>
@@ -19436,7 +19459,7 @@
       </c>
     </row>
     <row r="135" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A135" s="22"/>
+      <c r="A135" s="21"/>
       <c r="B135" s="5" t="s">
         <v>137</v>
       </c>
@@ -19568,7 +19591,7 @@
       </c>
     </row>
     <row r="136" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A136" s="22"/>
+      <c r="A136" s="21"/>
       <c r="B136" s="5" t="s">
         <v>138</v>
       </c>
@@ -19700,7 +19723,7 @@
       </c>
     </row>
     <row r="137" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A137" s="22"/>
+      <c r="A137" s="21"/>
       <c r="B137" s="5" t="s">
         <v>139</v>
       </c>
@@ -19832,7 +19855,7 @@
       </c>
     </row>
     <row r="138" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A138" s="22"/>
+      <c r="A138" s="21"/>
       <c r="B138" s="5" t="s">
         <v>140</v>
       </c>
@@ -19964,7 +19987,7 @@
       </c>
     </row>
     <row r="139" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A139" s="22"/>
+      <c r="A139" s="21"/>
       <c r="B139" s="5" t="s">
         <v>141</v>
       </c>
@@ -20096,7 +20119,7 @@
       </c>
     </row>
     <row r="140" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A140" s="22"/>
+      <c r="A140" s="21"/>
       <c r="B140" s="5" t="s">
         <v>142</v>
       </c>
@@ -20228,8 +20251,8 @@
       </c>
     </row>
     <row r="141" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A141" s="22" t="s">
-        <v>317</v>
+      <c r="A141" s="21" t="s">
+        <v>313</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>143</v>
@@ -20362,7 +20385,7 @@
       </c>
     </row>
     <row r="142" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A142" s="22"/>
+      <c r="A142" s="21"/>
       <c r="B142" s="5" t="s">
         <v>144</v>
       </c>
@@ -20494,7 +20517,7 @@
       </c>
     </row>
     <row r="143" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A143" s="22"/>
+      <c r="A143" s="21"/>
       <c r="B143" s="5" t="s">
         <v>145</v>
       </c>
@@ -20626,7 +20649,7 @@
       </c>
     </row>
     <row r="144" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A144" s="22"/>
+      <c r="A144" s="21"/>
       <c r="B144" s="5" t="s">
         <v>146</v>
       </c>
@@ -20758,7 +20781,7 @@
       </c>
     </row>
     <row r="145" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A145" s="22"/>
+      <c r="A145" s="21"/>
       <c r="B145" s="5" t="s">
         <v>147</v>
       </c>
@@ -20890,7 +20913,7 @@
       </c>
     </row>
     <row r="146" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A146" s="22"/>
+      <c r="A146" s="21"/>
       <c r="B146" s="5" t="s">
         <v>148</v>
       </c>
@@ -21022,7 +21045,7 @@
       </c>
     </row>
     <row r="147" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A147" s="22"/>
+      <c r="A147" s="21"/>
       <c r="B147" s="5" t="s">
         <v>149</v>
       </c>
@@ -21154,7 +21177,7 @@
       </c>
     </row>
     <row r="148" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A148" s="22"/>
+      <c r="A148" s="21"/>
       <c r="B148" s="5" t="s">
         <v>150</v>
       </c>
@@ -21286,8 +21309,8 @@
       </c>
     </row>
     <row r="149" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A149" s="22" t="s">
-        <v>319</v>
+      <c r="A149" s="21" t="s">
+        <v>315</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>151</v>
@@ -21420,7 +21443,7 @@
       </c>
     </row>
     <row r="150" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A150" s="22"/>
+      <c r="A150" s="21"/>
       <c r="B150" s="5" t="s">
         <v>152</v>
       </c>
@@ -21552,7 +21575,7 @@
       </c>
     </row>
     <row r="151" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A151" s="22"/>
+      <c r="A151" s="21"/>
       <c r="B151" s="5" t="s">
         <v>153</v>
       </c>
@@ -21562,8 +21585,8 @@
       <c r="D151" s="3">
         <v>2</v>
       </c>
-      <c r="E151" s="8">
-        <v>1</v>
+      <c r="E151" s="9">
+        <v>0</v>
       </c>
       <c r="F151" s="9">
         <v>0</v>
@@ -21571,8 +21594,8 @@
       <c r="G151" s="9">
         <v>0</v>
       </c>
-      <c r="H151" s="9">
-        <v>1</v>
+      <c r="H151" s="10">
+        <v>0</v>
       </c>
       <c r="I151" s="9">
         <v>0</v>
@@ -21684,7 +21707,7 @@
       </c>
     </row>
     <row r="152" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A152" s="22"/>
+      <c r="A152" s="21"/>
       <c r="B152" s="5" t="s">
         <v>154</v>
       </c>
@@ -21695,7 +21718,7 @@
         <v>3</v>
       </c>
       <c r="E152" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F152" s="9">
         <v>0</v>
@@ -21704,7 +21727,7 @@
         <v>0</v>
       </c>
       <c r="H152" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I152" s="9">
         <v>0</v>
@@ -21722,7 +21745,7 @@
         <v>0</v>
       </c>
       <c r="N152" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O152" s="9">
         <v>0</v>
@@ -21776,7 +21799,7 @@
         <v>0</v>
       </c>
       <c r="AF152" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG152" s="9">
         <v>0</v>
@@ -21797,7 +21820,7 @@
         <v>0</v>
       </c>
       <c r="AM152" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN152" s="9">
         <v>0</v>
@@ -21816,7 +21839,7 @@
       </c>
     </row>
     <row r="153" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A153" s="22"/>
+      <c r="A153" s="21"/>
       <c r="B153" s="5" t="s">
         <v>155</v>
       </c>
@@ -21948,7 +21971,7 @@
       </c>
     </row>
     <row r="154" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A154" s="22"/>
+      <c r="A154" s="21"/>
       <c r="B154" s="5" t="s">
         <v>156</v>
       </c>
@@ -22080,7 +22103,7 @@
       </c>
     </row>
     <row r="155" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A155" s="22"/>
+      <c r="A155" s="21"/>
       <c r="B155" s="5" t="s">
         <v>157</v>
       </c>
@@ -22212,7 +22235,7 @@
       </c>
     </row>
     <row r="156" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A156" s="22"/>
+      <c r="A156" s="21"/>
       <c r="B156" s="5" t="s">
         <v>158</v>
       </c>
@@ -22344,8 +22367,8 @@
       </c>
     </row>
     <row r="157" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A157" s="22" t="s">
-        <v>320</v>
+      <c r="A157" s="21" t="s">
+        <v>316</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>159</v>
@@ -22478,7 +22501,7 @@
       </c>
     </row>
     <row r="158" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A158" s="22"/>
+      <c r="A158" s="21"/>
       <c r="B158" s="5" t="s">
         <v>160</v>
       </c>
@@ -22610,7 +22633,7 @@
       </c>
     </row>
     <row r="159" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A159" s="22"/>
+      <c r="A159" s="21"/>
       <c r="B159" s="5" t="s">
         <v>161</v>
       </c>
@@ -22620,8 +22643,8 @@
       <c r="D159" s="3">
         <v>2</v>
       </c>
-      <c r="E159" s="8">
-        <v>1</v>
+      <c r="E159" s="9">
+        <v>0</v>
       </c>
       <c r="F159" s="9">
         <v>0</v>
@@ -22629,8 +22652,8 @@
       <c r="G159" s="9">
         <v>0</v>
       </c>
-      <c r="H159" s="9">
-        <v>1</v>
+      <c r="H159" s="10">
+        <v>0</v>
       </c>
       <c r="I159" s="9">
         <v>0</v>
@@ -22752,7 +22775,7 @@
         <v>3</v>
       </c>
       <c r="E160" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F160" s="9">
         <v>0</v>
@@ -22761,7 +22784,7 @@
         <v>0</v>
       </c>
       <c r="H160" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I160" s="9">
         <v>0</v>
@@ -22785,7 +22808,7 @@
         <v>0</v>
       </c>
       <c r="P160" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q160" s="9">
         <v>0</v>
@@ -22833,7 +22856,7 @@
         <v>0</v>
       </c>
       <c r="AF160" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG160" s="9">
         <v>0</v>
@@ -22854,7 +22877,7 @@
         <v>0</v>
       </c>
       <c r="AM160" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN160" s="9">
         <v>0</v>
@@ -23398,7 +23421,7 @@
     </row>
     <row r="165" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A165" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>167</v>
@@ -24449,7 +24472,7 @@
     </row>
     <row r="173" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A173" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>175</v>
@@ -25499,8 +25522,8 @@
       </c>
     </row>
     <row r="181" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A181" s="23" t="s">
-        <v>308</v>
+      <c r="A181" s="22" t="s">
+        <v>307</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>183</v>
@@ -26550,8 +26573,8 @@
       </c>
     </row>
     <row r="189" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A189" s="23" t="s">
-        <v>309</v>
+      <c r="A189" s="22" t="s">
+        <v>308</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>191</v>
@@ -27034,7 +27057,7 @@
         <v>0</v>
       </c>
       <c r="AE192" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF192" s="9">
         <v>0</v>
@@ -27162,7 +27185,7 @@
         <v>0</v>
       </c>
       <c r="AD193" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE193" s="9">
         <v>0</v>
@@ -27204,7 +27227,7 @@
         <v>0</v>
       </c>
       <c r="AR193" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:44" x14ac:dyDescent="0.3">
@@ -27323,7 +27346,7 @@
         <v>0</v>
       </c>
       <c r="AN194" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO194" s="9">
         <v>0</v>
@@ -27335,7 +27358,7 @@
         <v>0</v>
       </c>
       <c r="AR194" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:44" x14ac:dyDescent="0.3">
@@ -27348,119 +27371,119 @@
       <c r="D195" s="3">
         <v>6</v>
       </c>
-      <c r="E195" s="8">
+      <c r="E195" s="9">
+        <v>0</v>
+      </c>
+      <c r="F195" s="9">
+        <v>0</v>
+      </c>
+      <c r="G195" s="9">
+        <v>0</v>
+      </c>
+      <c r="H195" s="9">
+        <v>0</v>
+      </c>
+      <c r="I195" s="9">
+        <v>0</v>
+      </c>
+      <c r="J195" s="9">
+        <v>0</v>
+      </c>
+      <c r="K195" s="9">
+        <v>0</v>
+      </c>
+      <c r="L195" s="10">
+        <v>0</v>
+      </c>
+      <c r="M195" s="8">
+        <v>0</v>
+      </c>
+      <c r="N195" s="9">
+        <v>0</v>
+      </c>
+      <c r="O195" s="9">
+        <v>0</v>
+      </c>
+      <c r="P195" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q195" s="9">
+        <v>0</v>
+      </c>
+      <c r="R195" s="9">
+        <v>0</v>
+      </c>
+      <c r="S195" s="9">
+        <v>0</v>
+      </c>
+      <c r="T195" s="10">
+        <v>0</v>
+      </c>
+      <c r="U195" s="8">
+        <v>0</v>
+      </c>
+      <c r="V195" s="9">
+        <v>0</v>
+      </c>
+      <c r="W195" s="9">
+        <v>0</v>
+      </c>
+      <c r="X195" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y195" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB195" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC195" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ195" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK195" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN195" s="9">
         <v>1</v>
       </c>
-      <c r="F195" s="9">
-        <v>0</v>
-      </c>
-      <c r="G195" s="9">
-        <v>0</v>
-      </c>
-      <c r="H195" s="9">
-        <v>0</v>
-      </c>
-      <c r="I195" s="9">
-        <v>0</v>
-      </c>
-      <c r="J195" s="9">
+      <c r="AO195" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP195" s="9">
         <v>1</v>
-      </c>
-      <c r="K195" s="9">
-        <v>0</v>
-      </c>
-      <c r="L195" s="10">
-        <v>0</v>
-      </c>
-      <c r="M195" s="8">
-        <v>0</v>
-      </c>
-      <c r="N195" s="9">
-        <v>0</v>
-      </c>
-      <c r="O195" s="9">
-        <v>0</v>
-      </c>
-      <c r="P195" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q195" s="9">
-        <v>0</v>
-      </c>
-      <c r="R195" s="9">
-        <v>0</v>
-      </c>
-      <c r="S195" s="9">
-        <v>0</v>
-      </c>
-      <c r="T195" s="10">
-        <v>0</v>
-      </c>
-      <c r="U195" s="8">
-        <v>0</v>
-      </c>
-      <c r="V195" s="9">
-        <v>0</v>
-      </c>
-      <c r="W195" s="9">
-        <v>0</v>
-      </c>
-      <c r="X195" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y195" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB195" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC195" s="8">
-        <v>1</v>
-      </c>
-      <c r="AD195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ195" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK195" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AN195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AO195" s="9">
-        <v>0</v>
-      </c>
-      <c r="AP195" s="9">
-        <v>0</v>
       </c>
       <c r="AQ195" s="9">
         <v>0</v>
@@ -27480,7 +27503,7 @@
         <v>7</v>
       </c>
       <c r="E196" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F196" s="9">
         <v>0</v>
@@ -27495,7 +27518,7 @@
         <v>0</v>
       </c>
       <c r="J196" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K196" s="9">
         <v>0</v>
@@ -27552,7 +27575,7 @@
         <v>0</v>
       </c>
       <c r="AC196" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD196" s="9">
         <v>0</v>
@@ -27591,7 +27614,7 @@
         <v>0</v>
       </c>
       <c r="AP196" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ196" s="9">
         <v>0</v>
@@ -27601,7 +27624,7 @@
       </c>
     </row>
     <row r="197" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A197" s="21" t="s">
+      <c r="A197" s="22" t="s">
         <v>264</v>
       </c>
       <c r="B197" s="5" t="s">
@@ -27632,7 +27655,7 @@
         <v>0</v>
       </c>
       <c r="K197" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L197" s="10">
         <v>0</v>
@@ -27762,8 +27785,8 @@
       <c r="J198" s="9">
         <v>1</v>
       </c>
-      <c r="K198" s="9">
-        <v>1</v>
+      <c r="K198" s="10">
+        <v>0</v>
       </c>
       <c r="L198" s="10">
         <v>0</v>
@@ -35999,18 +36022,18 @@
     <mergeCell ref="U4:AB4"/>
     <mergeCell ref="AC4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:AJ148 E152:AJ156 E160:AJ180 E184:AJ1048576">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+  <conditionalFormatting sqref="E184:AJ189 E190:AD190 AF190:AJ190 E5:AJ30 I31:AJ31 I151:AJ151 E152:AJ158 I159:AJ159 E160:AJ180 I95:AJ95 E96:AJ150 E32:AJ94 E191:AJ194 F195:AJ195 E199:AJ1048576 E198:J198 L198:AJ198 E196:AJ197">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AJ4">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C1048576 C2:C3">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -36022,7 +36045,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D1048576 D2:D3">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -36034,41 +36057,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK5:AR148 AK152:AR156 AN149:AR151 AK160:AR180 AN157:AR159 AK184:AR1048576">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AR4">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E149:AJ151">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK149:AM151">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E157:AJ159">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK157:AM159">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E181:AJ183">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK181:AR183">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE190">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:H31">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151:H151">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E159:H159">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95:H95">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E195">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK181:AR183">
+  <conditionalFormatting sqref="K198">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed small ROM error
</commit_message>
<xml_diff>
--- a/ROMGeneration/MicroCodeRoms.xlsx
+++ b/ROMGeneration/MicroCodeRoms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\ROMGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF978F9-B30A-473D-9854-D90FF955EEC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A5CD7D-AC53-460C-8461-426A14FE264A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
   </bookViews>
   <sheets>
     <sheet name="ControlRoms" sheetId="1" r:id="rId1"/>
@@ -1871,8 +1871,8 @@
   <dimension ref="A1:AR260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
+      <pane ySplit="2" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K196" sqref="K196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27655,7 +27655,7 @@
         <v>0</v>
       </c>
       <c r="K197" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L197" s="10">
         <v>0</v>
@@ -27785,8 +27785,8 @@
       <c r="J198" s="9">
         <v>1</v>
       </c>
-      <c r="K198" s="10">
-        <v>0</v>
+      <c r="K198" s="9">
+        <v>1</v>
       </c>
       <c r="L198" s="10">
         <v>0</v>
@@ -36022,18 +36022,18 @@
     <mergeCell ref="U4:AB4"/>
     <mergeCell ref="AC4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E184:AJ189 E190:AD190 AF190:AJ190 E5:AJ30 I31:AJ31 I151:AJ151 E152:AJ158 I159:AJ159 E160:AJ180 I95:AJ95 E96:AJ150 E32:AJ94 E191:AJ194 F195:AJ195 E199:AJ1048576 E198:J198 L198:AJ198 E196:AJ197">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
+  <conditionalFormatting sqref="E184:AJ189 E190:AD190 AF190:AJ190 E5:AJ30 I31:AJ31 I151:AJ151 E152:AJ158 I159:AJ159 E160:AJ180 I95:AJ95 E96:AJ150 E32:AJ94 E191:AJ194 F195:AJ195 E196:AJ196 E197:J197 L197:AJ197 E198:AJ1048576">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AJ4">
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C1048576 C2:C3">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -36045,7 +36045,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D1048576 D2:D3">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -36057,66 +36057,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK5:AR148 AK152:AR156 AN149:AR151 AK160:AR180 AN157:AR159 AK184:AR1048576">
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AR4">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK149:AM151">
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK157:AM159">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E181:AJ183">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK181:AR183">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE190">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:H31">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E151:H151">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E159:H159">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95:H95">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E195">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K198">
+  <conditionalFormatting sqref="K197">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed POPM instruction not decrementing stackptr
</commit_message>
<xml_diff>
--- a/ROMGeneration/MicroCodeRoms.xlsx
+++ b/ROMGeneration/MicroCodeRoms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\ROMGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A227EE-2BF5-4926-84D0-7DF5DECD4846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A66A32C-F5CB-49D0-998C-2CB5DC1DFA51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
   </bookViews>
   <sheets>
     <sheet name="ControlRoms" sheetId="1" r:id="rId1"/>
@@ -1424,6 +1424,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1467,9 +1470,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2206,8 +2206,8 @@
   <dimension ref="A1:AR260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A252" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE245" sqref="AE245"/>
+      <pane ySplit="2" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P205" sqref="P205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2290,16 +2290,16 @@
       <c r="AR1" s="12"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -2424,10 +2424,10 @@
       </c>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="19">
         <v>0</v>
       </c>
@@ -2550,60 +2550,60 @@
       </c>
     </row>
     <row r="4" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="35" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="32" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="35" t="s">
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="32" t="s">
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="33"/>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="33"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="32" t="s">
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="AL4" s="33"/>
-      <c r="AM4" s="33"/>
-      <c r="AN4" s="33"/>
-      <c r="AO4" s="33"/>
-      <c r="AP4" s="33"/>
-      <c r="AQ4" s="33"/>
-      <c r="AR4" s="34"/>
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="34"/>
+      <c r="AO4" s="34"/>
+      <c r="AP4" s="34"/>
+      <c r="AQ4" s="34"/>
+      <c r="AR4" s="35"/>
     </row>
     <row r="5" spans="1:44" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
@@ -15302,7 +15302,7 @@
       </c>
     </row>
     <row r="101" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A101" s="38" t="s">
+      <c r="A101" s="23" t="s">
         <v>329</v>
       </c>
       <c r="B101" s="5" t="s">
@@ -29405,7 +29405,7 @@
         <v>0</v>
       </c>
       <c r="AQ207" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR207" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
Sub-Block Layout mostly finished
</commit_message>
<xml_diff>
--- a/ROMGeneration/MicroCodeRoms.xlsx
+++ b/ROMGeneration/MicroCodeRoms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\ROMGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A66A32C-F5CB-49D0-998C-2CB5DC1DFA51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59EAED0-0F80-4B17-BDC0-D76C1E493D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
   </bookViews>
   <sheets>
     <sheet name="ControlRoms" sheetId="1" r:id="rId1"/>
@@ -912,9 +912,6 @@
     <t>SUB</t>
   </si>
   <si>
-    <t>KOMPB</t>
-  </si>
-  <si>
     <t>NOTA</t>
   </si>
   <si>
@@ -1030,6 +1027,9 @@
   </si>
   <si>
     <t>ADDLB</t>
+  </si>
+  <si>
+    <t>COMPB</t>
   </si>
 </sst>
 </file>
@@ -2206,22 +2206,22 @@
   <dimension ref="A1:AR260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P205" sqref="P205"/>
+      <pane ySplit="2" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.3046875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.53515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="3" style="3" customWidth="1"/>
     <col min="5" max="5" width="3" style="8" customWidth="1"/>
     <col min="6" max="11" width="3" style="9" customWidth="1"/>
     <col min="12" max="12" width="3" style="10" customWidth="1"/>
     <col min="13" max="13" width="3" style="8" customWidth="1"/>
     <col min="14" max="15" width="3" style="9" customWidth="1"/>
-    <col min="16" max="16" width="2.88671875" style="9" customWidth="1"/>
+    <col min="16" max="16" width="2.84375" style="9" customWidth="1"/>
     <col min="17" max="19" width="3" style="9" customWidth="1"/>
     <col min="20" max="20" width="3" style="10" customWidth="1"/>
     <col min="21" max="21" width="3" style="8" customWidth="1"/>
@@ -2235,7 +2235,7 @@
     <col min="44" max="44" width="3" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="11">
         <v>4</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="AQ1" s="7"/>
       <c r="AR1" s="12"/>
     </row>
-    <row r="2" spans="1:44" s="1" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" s="1" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -2321,10 +2321,10 @@
         <v>267</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>271</v>
@@ -2351,7 +2351,7 @@
         <v>278</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>279</v>
@@ -2363,7 +2363,7 @@
         <v>284</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Z2" s="16" t="s">
         <v>280</v>
@@ -2390,40 +2390,40 @@
         <v>288</v>
       </c>
       <c r="AH2" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="AI2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="AJ2" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="AK2" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="AL2" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="AM2" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="AI2" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="AJ2" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="AK2" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="AL2" s="16" t="s">
+      <c r="AN2" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="AO2" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="AM2" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="AN2" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="AO2" s="17" t="s">
-        <v>306</v>
-      </c>
       <c r="AP2" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AQ2" s="17" t="s">
         <v>290</v>
       </c>
       <c r="AR2" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:44" s="1" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" s="1" customFormat="1" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25"/>
       <c r="B3" s="28"/>
       <c r="C3" s="31"/>
@@ -2549,7 +2549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="26"/>
       <c r="B4" s="29"/>
       <c r="C4" s="32"/>
@@ -2605,7 +2605,7 @@
       <c r="AQ4" s="34"/>
       <c r="AR4" s="35"/>
     </row>
-    <row r="5" spans="1:44" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A5" s="22" t="s">
         <v>263</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
@@ -2871,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
@@ -3003,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>9</v>
@@ -3135,7 +3135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>11</v>
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
       <c r="B10" s="5" t="s">
         <v>12</v>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
       <c r="B11" s="5" t="s">
         <v>13</v>
@@ -3531,7 +3531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>14</v>
@@ -3663,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A13" s="22" t="s">
         <v>270</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>16</v>
@@ -3929,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A15" s="21"/>
       <c r="B15" s="5" t="s">
         <v>17</v>
@@ -4061,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>18</v>
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A17" s="21"/>
       <c r="B17" s="5" t="s">
         <v>19</v>
@@ -4325,7 +4325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>20</v>
@@ -4457,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>21</v>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A20" s="21"/>
       <c r="B20" s="5" t="s">
         <v>22</v>
@@ -4721,7 +4721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
         <v>292</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>24</v>
@@ -4987,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A23" s="21"/>
       <c r="B23" s="5" t="s">
         <v>25</v>
@@ -5119,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>26</v>
@@ -5251,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A25" s="21"/>
       <c r="B25" s="5" t="s">
         <v>27</v>
@@ -5383,7 +5383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A26" s="21"/>
       <c r="B26" s="5" t="s">
         <v>28</v>
@@ -5515,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
         <v>29</v>
@@ -5647,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>30</v>
@@ -5779,9 +5779,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A29" s="22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>31</v>
@@ -5913,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>32</v>
@@ -6045,7 +6045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>33</v>
@@ -6177,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A32" s="21"/>
       <c r="B32" s="5" t="s">
         <v>34</v>
@@ -6309,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>35</v>
@@ -6441,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>36</v>
@@ -6573,7 +6573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A35" s="21"/>
       <c r="B35" s="5" t="s">
         <v>37</v>
@@ -6705,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A36" s="21"/>
       <c r="B36" s="5" t="s">
         <v>38</v>
@@ -6837,9 +6837,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A37" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>39</v>
@@ -6971,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A38" s="21"/>
       <c r="B38" s="5" t="s">
         <v>40</v>
@@ -7103,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A39" s="21"/>
       <c r="B39" s="5" t="s">
         <v>41</v>
@@ -7235,7 +7235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A40" s="21"/>
       <c r="B40" s="5" t="s">
         <v>42</v>
@@ -7367,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A41" s="21"/>
       <c r="B41" s="5" t="s">
         <v>43</v>
@@ -7499,7 +7499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A42" s="21"/>
       <c r="B42" s="5" t="s">
         <v>44</v>
@@ -7631,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A43" s="21"/>
       <c r="B43" s="5" t="s">
         <v>45</v>
@@ -7763,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A44" s="21"/>
       <c r="B44" s="5" t="s">
         <v>46</v>
@@ -7895,7 +7895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A45" s="22" t="s">
         <v>293</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A46" s="21"/>
       <c r="B46" s="5" t="s">
         <v>48</v>
@@ -8161,7 +8161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A47" s="21"/>
       <c r="B47" s="5" t="s">
         <v>49</v>
@@ -8293,7 +8293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A48" s="21"/>
       <c r="B48" s="5" t="s">
         <v>50</v>
@@ -8425,7 +8425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A49" s="21"/>
       <c r="B49" s="5" t="s">
         <v>51</v>
@@ -8557,7 +8557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A50" s="21"/>
       <c r="B50" s="5" t="s">
         <v>52</v>
@@ -8689,7 +8689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
         <v>53</v>
@@ -8821,7 +8821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A52" s="21"/>
       <c r="B52" s="5" t="s">
         <v>54</v>
@@ -8953,7 +8953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A53" s="22" t="s">
         <v>294</v>
       </c>
@@ -9087,7 +9087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A54" s="21"/>
       <c r="B54" s="5" t="s">
         <v>56</v>
@@ -9219,7 +9219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>57</v>
@@ -9351,7 +9351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
         <v>58</v>
@@ -9483,7 +9483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A57" s="21"/>
       <c r="B57" s="5" t="s">
         <v>59</v>
@@ -9615,7 +9615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A58" s="21"/>
       <c r="B58" s="5" t="s">
         <v>60</v>
@@ -9747,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A59" s="21"/>
       <c r="B59" s="5" t="s">
         <v>61</v>
@@ -9879,7 +9879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A60" s="21"/>
       <c r="B60" s="5" t="s">
         <v>62</v>
@@ -10011,9 +10011,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A61" s="22" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>63</v>
@@ -10145,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>64</v>
@@ -10277,7 +10277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>65</v>
@@ -10409,7 +10409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A64" s="21"/>
       <c r="B64" s="5" t="s">
         <v>66</v>
@@ -10541,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>67</v>
@@ -10673,7 +10673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>68</v>
@@ -10805,7 +10805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A67" s="21"/>
       <c r="B67" s="5" t="s">
         <v>69</v>
@@ -10937,7 +10937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A68" s="21"/>
       <c r="B68" s="5" t="s">
         <v>70</v>
@@ -11069,9 +11069,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A69" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>71</v>
@@ -11203,7 +11203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A70" s="21"/>
       <c r="B70" s="5" t="s">
         <v>72</v>
@@ -11335,7 +11335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A71" s="21"/>
       <c r="B71" s="5" t="s">
         <v>73</v>
@@ -11467,7 +11467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A72" s="21"/>
       <c r="B72" s="5" t="s">
         <v>74</v>
@@ -11599,7 +11599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A73" s="21"/>
       <c r="B73" s="5" t="s">
         <v>75</v>
@@ -11731,7 +11731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A74" s="21"/>
       <c r="B74" s="5" t="s">
         <v>76</v>
@@ -11863,7 +11863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A75" s="21"/>
       <c r="B75" s="5" t="s">
         <v>77</v>
@@ -11995,7 +11995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A76" s="21"/>
       <c r="B76" s="5" t="s">
         <v>78</v>
@@ -12127,9 +12127,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A77" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>79</v>
@@ -12261,7 +12261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A78" s="21"/>
       <c r="B78" s="5" t="s">
         <v>80</v>
@@ -12393,7 +12393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A79" s="21"/>
       <c r="B79" s="5" t="s">
         <v>81</v>
@@ -12525,7 +12525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A80" s="21"/>
       <c r="B80" s="5" t="s">
         <v>82</v>
@@ -12657,7 +12657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A81" s="21"/>
       <c r="B81" s="5" t="s">
         <v>83</v>
@@ -12789,7 +12789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A82" s="21"/>
       <c r="B82" s="5" t="s">
         <v>84</v>
@@ -12921,7 +12921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A83" s="21"/>
       <c r="B83" s="5" t="s">
         <v>85</v>
@@ -13053,7 +13053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A84" s="21"/>
       <c r="B84" s="5" t="s">
         <v>86</v>
@@ -13185,9 +13185,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A85" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>87</v>
@@ -13319,7 +13319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A86" s="21"/>
       <c r="B86" s="5" t="s">
         <v>88</v>
@@ -13451,7 +13451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A87" s="21"/>
       <c r="B87" s="5" t="s">
         <v>89</v>
@@ -13583,7 +13583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A88" s="21"/>
       <c r="B88" s="5" t="s">
         <v>90</v>
@@ -13715,7 +13715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A89" s="21"/>
       <c r="B89" s="5" t="s">
         <v>91</v>
@@ -13847,7 +13847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A90" s="21"/>
       <c r="B90" s="5" t="s">
         <v>92</v>
@@ -13979,7 +13979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A91" s="21"/>
       <c r="B91" s="5" t="s">
         <v>93</v>
@@ -14111,7 +14111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A92" s="21"/>
       <c r="B92" s="5" t="s">
         <v>94</v>
@@ -14243,9 +14243,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A93" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>95</v>
@@ -14377,7 +14377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A94" s="21"/>
       <c r="B94" s="5" t="s">
         <v>96</v>
@@ -14509,7 +14509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A95" s="21"/>
       <c r="B95" s="5" t="s">
         <v>97</v>
@@ -14641,7 +14641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A96" s="21"/>
       <c r="B96" s="5" t="s">
         <v>98</v>
@@ -14773,7 +14773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A97" s="21"/>
       <c r="B97" s="5" t="s">
         <v>99</v>
@@ -14905,7 +14905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A98" s="21"/>
       <c r="B98" s="5" t="s">
         <v>100</v>
@@ -15037,7 +15037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A99" s="21"/>
       <c r="B99" s="5" t="s">
         <v>101</v>
@@ -15169,7 +15169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A100" s="21"/>
       <c r="B100" s="5" t="s">
         <v>102</v>
@@ -15301,9 +15301,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A101" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>103</v>
@@ -15435,7 +15435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A102" s="21"/>
       <c r="B102" s="5" t="s">
         <v>104</v>
@@ -15567,7 +15567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A103" s="21"/>
       <c r="B103" s="5" t="s">
         <v>105</v>
@@ -15699,7 +15699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A104" s="21"/>
       <c r="B104" s="5" t="s">
         <v>106</v>
@@ -15831,7 +15831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A105" s="21"/>
       <c r="B105" s="5" t="s">
         <v>107</v>
@@ -15963,7 +15963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A106" s="21"/>
       <c r="B106" s="5" t="s">
         <v>108</v>
@@ -16095,7 +16095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A107" s="21"/>
       <c r="B107" s="5" t="s">
         <v>109</v>
@@ -16227,7 +16227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A108" s="21"/>
       <c r="B108" s="5" t="s">
         <v>110</v>
@@ -16359,9 +16359,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A109" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>111</v>
@@ -16493,7 +16493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A110" s="21"/>
       <c r="B110" s="5" t="s">
         <v>112</v>
@@ -16625,7 +16625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A111" s="21"/>
       <c r="B111" s="5" t="s">
         <v>113</v>
@@ -16757,7 +16757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A112" s="21"/>
       <c r="B112" s="5" t="s">
         <v>114</v>
@@ -16889,7 +16889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A113" s="21"/>
       <c r="B113" s="5" t="s">
         <v>115</v>
@@ -17021,7 +17021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A114" s="21"/>
       <c r="B114" s="5" t="s">
         <v>116</v>
@@ -17153,7 +17153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A115" s="21"/>
       <c r="B115" s="5" t="s">
         <v>117</v>
@@ -17285,7 +17285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A116" s="21"/>
       <c r="B116" s="5" t="s">
         <v>118</v>
@@ -17417,9 +17417,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A117" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>119</v>
@@ -17551,7 +17551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A118" s="21"/>
       <c r="B118" s="5" t="s">
         <v>120</v>
@@ -17683,7 +17683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A119" s="21"/>
       <c r="B119" s="5" t="s">
         <v>121</v>
@@ -17815,7 +17815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A120" s="21"/>
       <c r="B120" s="5" t="s">
         <v>122</v>
@@ -17947,7 +17947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A121" s="21"/>
       <c r="B121" s="5" t="s">
         <v>123</v>
@@ -18079,7 +18079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A122" s="21"/>
       <c r="B122" s="5" t="s">
         <v>124</v>
@@ -18211,7 +18211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A123" s="21"/>
       <c r="B123" s="5" t="s">
         <v>125</v>
@@ -18343,7 +18343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A124" s="21"/>
       <c r="B124" s="5" t="s">
         <v>126</v>
@@ -18475,9 +18475,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A125" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>127</v>
@@ -18609,7 +18609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A126" s="21"/>
       <c r="B126" s="5" t="s">
         <v>128</v>
@@ -18741,7 +18741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A127" s="21"/>
       <c r="B127" s="5" t="s">
         <v>129</v>
@@ -18873,7 +18873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A128" s="21"/>
       <c r="B128" s="5" t="s">
         <v>130</v>
@@ -19005,7 +19005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A129" s="21"/>
       <c r="B129" s="5" t="s">
         <v>131</v>
@@ -19137,7 +19137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A130" s="21"/>
       <c r="B130" s="5" t="s">
         <v>132</v>
@@ -19269,7 +19269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A131" s="21"/>
       <c r="B131" s="5" t="s">
         <v>133</v>
@@ -19401,7 +19401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A132" s="21"/>
       <c r="B132" s="5" t="s">
         <v>134</v>
@@ -19533,9 +19533,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A133" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>135</v>
@@ -19667,7 +19667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A134" s="21"/>
       <c r="B134" s="5" t="s">
         <v>136</v>
@@ -19799,7 +19799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A135" s="21"/>
       <c r="B135" s="5" t="s">
         <v>137</v>
@@ -19931,7 +19931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A136" s="21"/>
       <c r="B136" s="5" t="s">
         <v>138</v>
@@ -20063,7 +20063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A137" s="21"/>
       <c r="B137" s="5" t="s">
         <v>139</v>
@@ -20195,7 +20195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A138" s="21"/>
       <c r="B138" s="5" t="s">
         <v>140</v>
@@ -20327,7 +20327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A139" s="21"/>
       <c r="B139" s="5" t="s">
         <v>141</v>
@@ -20459,7 +20459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A140" s="21"/>
       <c r="B140" s="5" t="s">
         <v>142</v>
@@ -20591,9 +20591,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A141" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>143</v>
@@ -20725,7 +20725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A142" s="21"/>
       <c r="B142" s="5" t="s">
         <v>144</v>
@@ -20857,7 +20857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A143" s="21"/>
       <c r="B143" s="5" t="s">
         <v>145</v>
@@ -20989,7 +20989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A144" s="21"/>
       <c r="B144" s="5" t="s">
         <v>146</v>
@@ -21121,7 +21121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A145" s="21"/>
       <c r="B145" s="5" t="s">
         <v>147</v>
@@ -21253,7 +21253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A146" s="21"/>
       <c r="B146" s="5" t="s">
         <v>148</v>
@@ -21385,7 +21385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A147" s="21"/>
       <c r="B147" s="5" t="s">
         <v>149</v>
@@ -21517,7 +21517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A148" s="21"/>
       <c r="B148" s="5" t="s">
         <v>150</v>
@@ -21649,9 +21649,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A149" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>151</v>
@@ -21783,7 +21783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A150" s="21"/>
       <c r="B150" s="5" t="s">
         <v>152</v>
@@ -21915,7 +21915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A151" s="21"/>
       <c r="B151" s="5" t="s">
         <v>153</v>
@@ -22047,7 +22047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A152" s="21"/>
       <c r="B152" s="5" t="s">
         <v>154</v>
@@ -22179,7 +22179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A153" s="21"/>
       <c r="B153" s="5" t="s">
         <v>155</v>
@@ -22311,7 +22311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A154" s="21"/>
       <c r="B154" s="5" t="s">
         <v>156</v>
@@ -22443,7 +22443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A155" s="21"/>
       <c r="B155" s="5" t="s">
         <v>157</v>
@@ -22575,7 +22575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A156" s="21"/>
       <c r="B156" s="5" t="s">
         <v>158</v>
@@ -22707,9 +22707,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A157" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>159</v>
@@ -22841,7 +22841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A158" s="21"/>
       <c r="B158" s="5" t="s">
         <v>160</v>
@@ -22973,7 +22973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A159" s="21"/>
       <c r="B159" s="5" t="s">
         <v>161</v>
@@ -23105,7 +23105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B160" s="5" t="s">
         <v>162</v>
       </c>
@@ -23236,7 +23236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B161" s="5" t="s">
         <v>163</v>
       </c>
@@ -23367,7 +23367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B162" s="5" t="s">
         <v>164</v>
       </c>
@@ -23498,7 +23498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B163" s="5" t="s">
         <v>165</v>
       </c>
@@ -23629,7 +23629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B164" s="5" t="s">
         <v>166</v>
       </c>
@@ -23760,9 +23760,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A165" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>167</v>
@@ -23894,7 +23894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B166" s="5" t="s">
         <v>168</v>
       </c>
@@ -24025,7 +24025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B167" s="5" t="s">
         <v>169</v>
       </c>
@@ -24156,7 +24156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B168" s="5" t="s">
         <v>170</v>
       </c>
@@ -24287,7 +24287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B169" s="5" t="s">
         <v>171</v>
       </c>
@@ -24418,7 +24418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B170" s="5" t="s">
         <v>172</v>
       </c>
@@ -24549,7 +24549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B171" s="5" t="s">
         <v>173</v>
       </c>
@@ -24680,7 +24680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B172" s="5" t="s">
         <v>174</v>
       </c>
@@ -24811,9 +24811,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A173" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>175</v>
@@ -24945,7 +24945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B174" s="5" t="s">
         <v>176</v>
       </c>
@@ -25076,7 +25076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B175" s="5" t="s">
         <v>177</v>
       </c>
@@ -25207,7 +25207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B176" s="5" t="s">
         <v>178</v>
       </c>
@@ -25338,7 +25338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B177" s="5" t="s">
         <v>179</v>
       </c>
@@ -25469,7 +25469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B178" s="5" t="s">
         <v>180</v>
       </c>
@@ -25600,7 +25600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B179" s="5" t="s">
         <v>181</v>
       </c>
@@ -25731,7 +25731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B180" s="5" t="s">
         <v>182</v>
       </c>
@@ -25862,9 +25862,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A181" s="22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>183</v>
@@ -25996,7 +25996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B182" s="5" t="s">
         <v>184</v>
       </c>
@@ -26127,7 +26127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B183" s="5" t="s">
         <v>185</v>
       </c>
@@ -26258,7 +26258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B184" s="5" t="s">
         <v>186</v>
       </c>
@@ -26389,7 +26389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B185" s="5" t="s">
         <v>187</v>
       </c>
@@ -26520,7 +26520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B186" s="5" t="s">
         <v>188</v>
       </c>
@@ -26651,7 +26651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B187" s="5" t="s">
         <v>189</v>
       </c>
@@ -26782,7 +26782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B188" s="5" t="s">
         <v>190</v>
       </c>
@@ -26913,9 +26913,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A189" s="22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>191</v>
@@ -27047,7 +27047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B190" s="5" t="s">
         <v>192</v>
       </c>
@@ -27178,7 +27178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B191" s="5" t="s">
         <v>193</v>
       </c>
@@ -27309,7 +27309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B192" s="5" t="s">
         <v>194</v>
       </c>
@@ -27440,7 +27440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B193" s="5" t="s">
         <v>195</v>
       </c>
@@ -27571,7 +27571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B194" s="5" t="s">
         <v>196</v>
       </c>
@@ -27702,7 +27702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B195" s="5" t="s">
         <v>197</v>
       </c>
@@ -27833,7 +27833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B196" s="5" t="s">
         <v>198</v>
       </c>
@@ -27964,9 +27964,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A197" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>199</v>
@@ -28098,7 +28098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B198" s="5" t="s">
         <v>200</v>
       </c>
@@ -28229,7 +28229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B199" s="5" t="s">
         <v>201</v>
       </c>
@@ -28360,7 +28360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B200" s="5" t="s">
         <v>202</v>
       </c>
@@ -28491,7 +28491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B201" s="5" t="s">
         <v>203</v>
       </c>
@@ -28622,7 +28622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B202" s="5" t="s">
         <v>204</v>
       </c>
@@ -28753,7 +28753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B203" s="5" t="s">
         <v>205</v>
       </c>
@@ -28884,7 +28884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B204" s="5" t="s">
         <v>206</v>
       </c>
@@ -29015,9 +29015,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A205" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B205" s="5" t="s">
         <v>207</v>
@@ -29149,7 +29149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B206" s="5" t="s">
         <v>208</v>
       </c>
@@ -29280,7 +29280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B207" s="5" t="s">
         <v>209</v>
       </c>
@@ -29411,7 +29411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B208" s="5" t="s">
         <v>210</v>
       </c>
@@ -29542,7 +29542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B209" s="5" t="s">
         <v>211</v>
       </c>
@@ -29673,7 +29673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B210" s="5" t="s">
         <v>212</v>
       </c>
@@ -29804,7 +29804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B211" s="5" t="s">
         <v>213</v>
       </c>
@@ -29935,7 +29935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B212" s="5" t="s">
         <v>214</v>
       </c>
@@ -30066,9 +30066,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A213" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B213" s="5" t="s">
         <v>215</v>
@@ -30200,7 +30200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B214" s="5" t="s">
         <v>216</v>
       </c>
@@ -30331,7 +30331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B215" s="5" t="s">
         <v>217</v>
       </c>
@@ -30462,7 +30462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B216" s="5" t="s">
         <v>218</v>
       </c>
@@ -30593,7 +30593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B217" s="5" t="s">
         <v>219</v>
       </c>
@@ -30724,7 +30724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B218" s="5" t="s">
         <v>220</v>
       </c>
@@ -30855,7 +30855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B219" s="5" t="s">
         <v>221</v>
       </c>
@@ -30986,7 +30986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B220" s="5" t="s">
         <v>222</v>
       </c>
@@ -31117,9 +31117,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A221" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B221" s="5" t="s">
         <v>223</v>
@@ -31251,7 +31251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B222" s="5" t="s">
         <v>224</v>
       </c>
@@ -31382,7 +31382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B223" s="5" t="s">
         <v>225</v>
       </c>
@@ -31513,7 +31513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B224" s="5" t="s">
         <v>226</v>
       </c>
@@ -31644,7 +31644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B225" s="5" t="s">
         <v>227</v>
       </c>
@@ -31775,7 +31775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B226" s="5" t="s">
         <v>228</v>
       </c>
@@ -31906,7 +31906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B227" s="5" t="s">
         <v>229</v>
       </c>
@@ -32037,7 +32037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B228" s="5" t="s">
         <v>230</v>
       </c>
@@ -32168,9 +32168,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A229" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B229" s="5" t="s">
         <v>231</v>
@@ -32302,7 +32302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B230" s="5" t="s">
         <v>232</v>
       </c>
@@ -32433,7 +32433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B231" s="5" t="s">
         <v>233</v>
       </c>
@@ -32564,7 +32564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B232" s="5" t="s">
         <v>234</v>
       </c>
@@ -32695,7 +32695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B233" s="5" t="s">
         <v>235</v>
       </c>
@@ -32826,7 +32826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B234" s="5" t="s">
         <v>236</v>
       </c>
@@ -32957,7 +32957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B235" s="5" t="s">
         <v>237</v>
       </c>
@@ -33088,7 +33088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B236" s="5" t="s">
         <v>238</v>
       </c>
@@ -33219,9 +33219,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A237" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B237" s="5" t="s">
         <v>239</v>
@@ -33353,7 +33353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B238" s="5" t="s">
         <v>240</v>
       </c>
@@ -33484,7 +33484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B239" s="5" t="s">
         <v>241</v>
       </c>
@@ -33615,7 +33615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B240" s="5" t="s">
         <v>242</v>
       </c>
@@ -33746,7 +33746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B241" s="5" t="s">
         <v>243</v>
       </c>
@@ -33877,7 +33877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B242" s="5" t="s">
         <v>244</v>
       </c>
@@ -34008,7 +34008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B243" s="5" t="s">
         <v>245</v>
       </c>
@@ -34139,7 +34139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B244" s="5" t="s">
         <v>246</v>
       </c>
@@ -34270,7 +34270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A245" s="22" t="s">
         <v>264</v>
       </c>
@@ -34404,7 +34404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B246" s="5" t="s">
         <v>248</v>
       </c>
@@ -34535,7 +34535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B247" s="5" t="s">
         <v>249</v>
       </c>
@@ -34666,7 +34666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B248" s="5" t="s">
         <v>250</v>
       </c>
@@ -34797,7 +34797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B249" s="5" t="s">
         <v>251</v>
       </c>
@@ -34928,7 +34928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B250" s="5" t="s">
         <v>252</v>
       </c>
@@ -35059,7 +35059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B251" s="5" t="s">
         <v>253</v>
       </c>
@@ -35190,7 +35190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B252" s="5" t="s">
         <v>254</v>
       </c>
@@ -35321,9 +35321,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:44" x14ac:dyDescent="0.4">
       <c r="A253" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B253" s="5" t="s">
         <v>255</v>
@@ -35455,7 +35455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B254" s="5" t="s">
         <v>256</v>
       </c>
@@ -35586,7 +35586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B255" s="5" t="s">
         <v>257</v>
       </c>
@@ -35717,7 +35717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:44" x14ac:dyDescent="0.4">
       <c r="B256" s="5" t="s">
         <v>258</v>
       </c>
@@ -35848,7 +35848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:44" x14ac:dyDescent="0.4">
       <c r="B257" s="5" t="s">
         <v>259</v>
       </c>
@@ -35979,7 +35979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:44" x14ac:dyDescent="0.4">
       <c r="B258" s="5" t="s">
         <v>260</v>
       </c>
@@ -36110,7 +36110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:44" x14ac:dyDescent="0.4">
       <c r="B259" s="5" t="s">
         <v>261</v>
       </c>
@@ -36241,7 +36241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="2:44" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:44" x14ac:dyDescent="0.4">
       <c r="B260" s="5" t="s">
         <v>262</v>
       </c>

</xml_diff>

<commit_message>
Logisim: Interrupts updated, now work with new clk
</commit_message>
<xml_diff>
--- a/ROMGeneration/MicroCodeRoms.xlsx
+++ b/ROMGeneration/MicroCodeRoms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pschilk\home\Repos\psMCU\ROMGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59EAED0-0F80-4B17-BDC0-D76C1E493D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3264418-00E7-44D7-99C1-4C689C5F61E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{29B2112A-6599-40BB-9E31-9AC80386968F}"/>
   </bookViews>
   <sheets>
     <sheet name="ControlRoms" sheetId="1" r:id="rId1"/>
@@ -984,12 +984,6 @@
     <t>RTRNI</t>
   </si>
   <si>
-    <t>INT_Reset</t>
-  </si>
-  <si>
-    <t>INT_Set</t>
-  </si>
-  <si>
     <t>ALU_DoBComp</t>
   </si>
   <si>
@@ -1030,6 +1024,12 @@
   </si>
   <si>
     <t>COMPB</t>
+  </si>
+  <si>
+    <t>Int Override Clr</t>
+  </si>
+  <si>
+    <t>Int Clr</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1476,28 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="62">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2206,22 +2227,22 @@
   <dimension ref="A1:AR260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="2" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O258" sqref="O258"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.3046875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="5.53515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" style="4" customWidth="1"/>
     <col min="4" max="4" width="3" style="3" customWidth="1"/>
     <col min="5" max="5" width="3" style="8" customWidth="1"/>
     <col min="6" max="11" width="3" style="9" customWidth="1"/>
     <col min="12" max="12" width="3" style="10" customWidth="1"/>
     <col min="13" max="13" width="3" style="8" customWidth="1"/>
     <col min="14" max="15" width="3" style="9" customWidth="1"/>
-    <col min="16" max="16" width="2.84375" style="9" customWidth="1"/>
+    <col min="16" max="16" width="2.81640625" style="9" customWidth="1"/>
     <col min="17" max="19" width="3" style="9" customWidth="1"/>
     <col min="20" max="20" width="3" style="10" customWidth="1"/>
     <col min="21" max="21" width="3" style="8" customWidth="1"/>
@@ -2235,7 +2256,7 @@
     <col min="44" max="44" width="3" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11">
         <v>4</v>
       </c>
@@ -2289,7 +2310,7 @@
       <c r="AQ1" s="7"/>
       <c r="AR1" s="12"/>
     </row>
-    <row r="2" spans="1:44" s="1" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:44" s="1" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -2324,7 +2345,7 @@
         <v>310</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>271</v>
@@ -2351,7 +2372,7 @@
         <v>278</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>279</v>
@@ -2396,7 +2417,7 @@
         <v>317</v>
       </c>
       <c r="AJ2" s="18" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="AK2" s="15" t="s">
         <v>315</v>
@@ -2423,7 +2444,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:44" s="1" customFormat="1" ht="16.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:44" s="1" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25"/>
       <c r="B3" s="28"/>
       <c r="C3" s="31"/>
@@ -2549,7 +2570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="26"/>
       <c r="B4" s="29"/>
       <c r="C4" s="32"/>
@@ -2605,7 +2626,7 @@
       <c r="AQ4" s="34"/>
       <c r="AR4" s="35"/>
     </row>
-    <row r="5" spans="1:44" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:44" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>263</v>
       </c>
@@ -2739,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
@@ -2871,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="21"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
@@ -3003,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
       <c r="B8" s="5" t="s">
         <v>9</v>
@@ -3135,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
       <c r="B9" s="5" t="s">
         <v>11</v>
@@ -3267,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="5" t="s">
         <v>12</v>
@@ -3399,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
       <c r="B11" s="5" t="s">
         <v>13</v>
@@ -3531,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" s="21"/>
       <c r="B12" s="5" t="s">
         <v>14</v>
@@ -3663,7 +3684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>270</v>
       </c>
@@ -3797,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
       <c r="B14" s="5" t="s">
         <v>16</v>
@@ -3808,8 +3829,8 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="8">
-        <v>1</v>
+      <c r="E14" s="9">
+        <v>0</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
@@ -3818,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="9">
         <v>0</v>
@@ -3929,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
       <c r="B15" s="5" t="s">
         <v>17</v>
@@ -3941,7 +3962,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="9">
         <v>0</v>
@@ -3950,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="9">
         <v>0</v>
@@ -4061,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
       <c r="B16" s="5" t="s">
         <v>18</v>
@@ -4193,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
       <c r="B17" s="5" t="s">
         <v>19</v>
@@ -4325,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A18" s="21"/>
       <c r="B18" s="5" t="s">
         <v>20</v>
@@ -4457,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A19" s="21"/>
       <c r="B19" s="5" t="s">
         <v>21</v>
@@ -4589,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A20" s="21"/>
       <c r="B20" s="5" t="s">
         <v>22</v>
@@ -4721,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>292</v>
       </c>
@@ -4855,7 +4876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A22" s="21"/>
       <c r="B22" s="5" t="s">
         <v>24</v>
@@ -4987,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A23" s="21"/>
       <c r="B23" s="5" t="s">
         <v>25</v>
@@ -5119,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
       <c r="B24" s="5" t="s">
         <v>26</v>
@@ -5251,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A25" s="21"/>
       <c r="B25" s="5" t="s">
         <v>27</v>
@@ -5383,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A26" s="21"/>
       <c r="B26" s="5" t="s">
         <v>28</v>
@@ -5515,7 +5536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A27" s="21"/>
       <c r="B27" s="5" t="s">
         <v>29</v>
@@ -5647,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A28" s="21"/>
       <c r="B28" s="5" t="s">
         <v>30</v>
@@ -5779,9 +5800,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>31</v>
@@ -5913,7 +5934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A30" s="21"/>
       <c r="B30" s="5" t="s">
         <v>32</v>
@@ -6045,7 +6066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A31" s="21"/>
       <c r="B31" s="5" t="s">
         <v>33</v>
@@ -6177,7 +6198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A32" s="21"/>
       <c r="B32" s="5" t="s">
         <v>34</v>
@@ -6309,7 +6330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>35</v>
@@ -6441,7 +6462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>36</v>
@@ -6573,7 +6594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A35" s="21"/>
       <c r="B35" s="5" t="s">
         <v>37</v>
@@ -6705,7 +6726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A36" s="21"/>
       <c r="B36" s="5" t="s">
         <v>38</v>
@@ -6837,9 +6858,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>39</v>
@@ -6971,7 +6992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A38" s="21"/>
       <c r="B38" s="5" t="s">
         <v>40</v>
@@ -7103,7 +7124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A39" s="21"/>
       <c r="B39" s="5" t="s">
         <v>41</v>
@@ -7235,7 +7256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A40" s="21"/>
       <c r="B40" s="5" t="s">
         <v>42</v>
@@ -7367,7 +7388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A41" s="21"/>
       <c r="B41" s="5" t="s">
         <v>43</v>
@@ -7499,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A42" s="21"/>
       <c r="B42" s="5" t="s">
         <v>44</v>
@@ -7631,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A43" s="21"/>
       <c r="B43" s="5" t="s">
         <v>45</v>
@@ -7763,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A44" s="21"/>
       <c r="B44" s="5" t="s">
         <v>46</v>
@@ -7895,7 +7916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A45" s="22" t="s">
         <v>293</v>
       </c>
@@ -8029,7 +8050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A46" s="21"/>
       <c r="B46" s="5" t="s">
         <v>48</v>
@@ -8161,7 +8182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A47" s="21"/>
       <c r="B47" s="5" t="s">
         <v>49</v>
@@ -8293,7 +8314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A48" s="21"/>
       <c r="B48" s="5" t="s">
         <v>50</v>
@@ -8425,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A49" s="21"/>
       <c r="B49" s="5" t="s">
         <v>51</v>
@@ -8557,7 +8578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A50" s="21"/>
       <c r="B50" s="5" t="s">
         <v>52</v>
@@ -8689,7 +8710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A51" s="21"/>
       <c r="B51" s="5" t="s">
         <v>53</v>
@@ -8821,7 +8842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A52" s="21"/>
       <c r="B52" s="5" t="s">
         <v>54</v>
@@ -8953,7 +8974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A53" s="22" t="s">
         <v>294</v>
       </c>
@@ -9087,7 +9108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A54" s="21"/>
       <c r="B54" s="5" t="s">
         <v>56</v>
@@ -9219,7 +9240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>57</v>
@@ -9351,7 +9372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
         <v>58</v>
@@ -9483,7 +9504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A57" s="21"/>
       <c r="B57" s="5" t="s">
         <v>59</v>
@@ -9615,7 +9636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A58" s="21"/>
       <c r="B58" s="5" t="s">
         <v>60</v>
@@ -9747,7 +9768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A59" s="21"/>
       <c r="B59" s="5" t="s">
         <v>61</v>
@@ -9879,7 +9900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A60" s="21"/>
       <c r="B60" s="5" t="s">
         <v>62</v>
@@ -10011,9 +10032,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A61" s="22" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>63</v>
@@ -10145,7 +10166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>64</v>
@@ -10277,7 +10298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>65</v>
@@ -10409,7 +10430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A64" s="21"/>
       <c r="B64" s="5" t="s">
         <v>66</v>
@@ -10541,7 +10562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>67</v>
@@ -10673,7 +10694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>68</v>
@@ -10805,7 +10826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A67" s="21"/>
       <c r="B67" s="5" t="s">
         <v>69</v>
@@ -10937,7 +10958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A68" s="21"/>
       <c r="B68" s="5" t="s">
         <v>70</v>
@@ -11069,7 +11090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A69" s="22" t="s">
         <v>295</v>
       </c>
@@ -11203,7 +11224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A70" s="21"/>
       <c r="B70" s="5" t="s">
         <v>72</v>
@@ -11335,7 +11356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A71" s="21"/>
       <c r="B71" s="5" t="s">
         <v>73</v>
@@ -11467,7 +11488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A72" s="21"/>
       <c r="B72" s="5" t="s">
         <v>74</v>
@@ -11599,7 +11620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A73" s="21"/>
       <c r="B73" s="5" t="s">
         <v>75</v>
@@ -11731,7 +11752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A74" s="21"/>
       <c r="B74" s="5" t="s">
         <v>76</v>
@@ -11863,7 +11884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A75" s="21"/>
       <c r="B75" s="5" t="s">
         <v>77</v>
@@ -11995,7 +12016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A76" s="21"/>
       <c r="B76" s="5" t="s">
         <v>78</v>
@@ -12127,7 +12148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A77" s="22" t="s">
         <v>296</v>
       </c>
@@ -12261,7 +12282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A78" s="21"/>
       <c r="B78" s="5" t="s">
         <v>80</v>
@@ -12393,7 +12414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A79" s="21"/>
       <c r="B79" s="5" t="s">
         <v>81</v>
@@ -12525,7 +12546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A80" s="21"/>
       <c r="B80" s="5" t="s">
         <v>82</v>
@@ -12657,7 +12678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A81" s="21"/>
       <c r="B81" s="5" t="s">
         <v>83</v>
@@ -12789,7 +12810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A82" s="21"/>
       <c r="B82" s="5" t="s">
         <v>84</v>
@@ -12921,7 +12942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A83" s="21"/>
       <c r="B83" s="5" t="s">
         <v>85</v>
@@ -13053,7 +13074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A84" s="21"/>
       <c r="B84" s="5" t="s">
         <v>86</v>
@@ -13185,9 +13206,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A85" s="22" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>87</v>
@@ -13319,7 +13340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A86" s="21"/>
       <c r="B86" s="5" t="s">
         <v>88</v>
@@ -13451,7 +13472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A87" s="21"/>
       <c r="B87" s="5" t="s">
         <v>89</v>
@@ -13583,7 +13604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A88" s="21"/>
       <c r="B88" s="5" t="s">
         <v>90</v>
@@ -13715,7 +13736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A89" s="21"/>
       <c r="B89" s="5" t="s">
         <v>91</v>
@@ -13847,7 +13868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A90" s="21"/>
       <c r="B90" s="5" t="s">
         <v>92</v>
@@ -13979,7 +14000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A91" s="21"/>
       <c r="B91" s="5" t="s">
         <v>93</v>
@@ -14111,7 +14132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A92" s="21"/>
       <c r="B92" s="5" t="s">
         <v>94</v>
@@ -14243,9 +14264,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A93" s="22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>95</v>
@@ -14377,7 +14398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A94" s="21"/>
       <c r="B94" s="5" t="s">
         <v>96</v>
@@ -14509,7 +14530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A95" s="21"/>
       <c r="B95" s="5" t="s">
         <v>97</v>
@@ -14641,7 +14662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A96" s="21"/>
       <c r="B96" s="5" t="s">
         <v>98</v>
@@ -14773,7 +14794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A97" s="21"/>
       <c r="B97" s="5" t="s">
         <v>99</v>
@@ -14905,7 +14926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A98" s="21"/>
       <c r="B98" s="5" t="s">
         <v>100</v>
@@ -15037,7 +15058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A99" s="21"/>
       <c r="B99" s="5" t="s">
         <v>101</v>
@@ -15169,7 +15190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A100" s="21"/>
       <c r="B100" s="5" t="s">
         <v>102</v>
@@ -15301,9 +15322,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A101" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>103</v>
@@ -15435,7 +15456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A102" s="21"/>
       <c r="B102" s="5" t="s">
         <v>104</v>
@@ -15567,7 +15588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A103" s="21"/>
       <c r="B103" s="5" t="s">
         <v>105</v>
@@ -15699,7 +15720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A104" s="21"/>
       <c r="B104" s="5" t="s">
         <v>106</v>
@@ -15831,7 +15852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A105" s="21"/>
       <c r="B105" s="5" t="s">
         <v>107</v>
@@ -15963,7 +15984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A106" s="21"/>
       <c r="B106" s="5" t="s">
         <v>108</v>
@@ -16095,7 +16116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A107" s="21"/>
       <c r="B107" s="5" t="s">
         <v>109</v>
@@ -16227,7 +16248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A108" s="21"/>
       <c r="B108" s="5" t="s">
         <v>110</v>
@@ -16359,7 +16380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A109" s="22" t="s">
         <v>297</v>
       </c>
@@ -16493,7 +16514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A110" s="21"/>
       <c r="B110" s="5" t="s">
         <v>112</v>
@@ -16625,7 +16646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A111" s="21"/>
       <c r="B111" s="5" t="s">
         <v>113</v>
@@ -16757,7 +16778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A112" s="21"/>
       <c r="B112" s="5" t="s">
         <v>114</v>
@@ -16889,7 +16910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A113" s="21"/>
       <c r="B113" s="5" t="s">
         <v>115</v>
@@ -17021,7 +17042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A114" s="21"/>
       <c r="B114" s="5" t="s">
         <v>116</v>
@@ -17153,7 +17174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A115" s="21"/>
       <c r="B115" s="5" t="s">
         <v>117</v>
@@ -17285,7 +17306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A116" s="21"/>
       <c r="B116" s="5" t="s">
         <v>118</v>
@@ -17417,7 +17438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A117" s="22" t="s">
         <v>298</v>
       </c>
@@ -17551,7 +17572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A118" s="21"/>
       <c r="B118" s="5" t="s">
         <v>120</v>
@@ -17683,7 +17704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A119" s="21"/>
       <c r="B119" s="5" t="s">
         <v>121</v>
@@ -17815,7 +17836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A120" s="21"/>
       <c r="B120" s="5" t="s">
         <v>122</v>
@@ -17947,7 +17968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A121" s="21"/>
       <c r="B121" s="5" t="s">
         <v>123</v>
@@ -18079,7 +18100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A122" s="21"/>
       <c r="B122" s="5" t="s">
         <v>124</v>
@@ -18211,7 +18232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A123" s="21"/>
       <c r="B123" s="5" t="s">
         <v>125</v>
@@ -18343,7 +18364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A124" s="21"/>
       <c r="B124" s="5" t="s">
         <v>126</v>
@@ -18475,7 +18496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A125" s="22" t="s">
         <v>299</v>
       </c>
@@ -18609,7 +18630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A126" s="21"/>
       <c r="B126" s="5" t="s">
         <v>128</v>
@@ -18741,7 +18762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A127" s="21"/>
       <c r="B127" s="5" t="s">
         <v>129</v>
@@ -18873,7 +18894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A128" s="21"/>
       <c r="B128" s="5" t="s">
         <v>130</v>
@@ -19005,7 +19026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A129" s="21"/>
       <c r="B129" s="5" t="s">
         <v>131</v>
@@ -19137,7 +19158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A130" s="21"/>
       <c r="B130" s="5" t="s">
         <v>132</v>
@@ -19269,7 +19290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A131" s="21"/>
       <c r="B131" s="5" t="s">
         <v>133</v>
@@ -19401,7 +19422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A132" s="21"/>
       <c r="B132" s="5" t="s">
         <v>134</v>
@@ -19533,7 +19554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A133" s="22" t="s">
         <v>307</v>
       </c>
@@ -19667,7 +19688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A134" s="21"/>
       <c r="B134" s="5" t="s">
         <v>136</v>
@@ -19799,7 +19820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A135" s="21"/>
       <c r="B135" s="5" t="s">
         <v>137</v>
@@ -19931,7 +19952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A136" s="21"/>
       <c r="B136" s="5" t="s">
         <v>138</v>
@@ -20063,7 +20084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A137" s="21"/>
       <c r="B137" s="5" t="s">
         <v>139</v>
@@ -20195,7 +20216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A138" s="21"/>
       <c r="B138" s="5" t="s">
         <v>140</v>
@@ -20327,7 +20348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A139" s="21"/>
       <c r="B139" s="5" t="s">
         <v>141</v>
@@ -20459,7 +20480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A140" s="21"/>
       <c r="B140" s="5" t="s">
         <v>142</v>
@@ -20591,7 +20612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A141" s="22" t="s">
         <v>306</v>
       </c>
@@ -20725,7 +20746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A142" s="21"/>
       <c r="B142" s="5" t="s">
         <v>144</v>
@@ -20857,7 +20878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A143" s="21"/>
       <c r="B143" s="5" t="s">
         <v>145</v>
@@ -20989,7 +21010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A144" s="21"/>
       <c r="B144" s="5" t="s">
         <v>146</v>
@@ -21121,7 +21142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A145" s="21"/>
       <c r="B145" s="5" t="s">
         <v>147</v>
@@ -21253,7 +21274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A146" s="21"/>
       <c r="B146" s="5" t="s">
         <v>148</v>
@@ -21385,7 +21406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A147" s="21"/>
       <c r="B147" s="5" t="s">
         <v>149</v>
@@ -21517,7 +21538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A148" s="21"/>
       <c r="B148" s="5" t="s">
         <v>150</v>
@@ -21649,7 +21670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A149" s="22" t="s">
         <v>308</v>
       </c>
@@ -21783,7 +21804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A150" s="21"/>
       <c r="B150" s="5" t="s">
         <v>152</v>
@@ -21915,7 +21936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A151" s="21"/>
       <c r="B151" s="5" t="s">
         <v>153</v>
@@ -22047,7 +22068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A152" s="21"/>
       <c r="B152" s="5" t="s">
         <v>154</v>
@@ -22179,7 +22200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A153" s="21"/>
       <c r="B153" s="5" t="s">
         <v>155</v>
@@ -22311,7 +22332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A154" s="21"/>
       <c r="B154" s="5" t="s">
         <v>156</v>
@@ -22443,7 +22464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A155" s="21"/>
       <c r="B155" s="5" t="s">
         <v>157</v>
@@ -22575,7 +22596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A156" s="21"/>
       <c r="B156" s="5" t="s">
         <v>158</v>
@@ -22707,7 +22728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A157" s="22" t="s">
         <v>309</v>
       </c>
@@ -22841,7 +22862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A158" s="21"/>
       <c r="B158" s="5" t="s">
         <v>160</v>
@@ -22973,7 +22994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A159" s="21"/>
       <c r="B159" s="5" t="s">
         <v>161</v>
@@ -23105,7 +23126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B160" s="5" t="s">
         <v>162</v>
       </c>
@@ -23236,7 +23257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B161" s="5" t="s">
         <v>163</v>
       </c>
@@ -23367,7 +23388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B162" s="5" t="s">
         <v>164</v>
       </c>
@@ -23498,7 +23519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B163" s="5" t="s">
         <v>165</v>
       </c>
@@ -23629,7 +23650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B164" s="5" t="s">
         <v>166</v>
       </c>
@@ -23760,7 +23781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A165" s="22" t="s">
         <v>300</v>
       </c>
@@ -23894,7 +23915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B166" s="5" t="s">
         <v>168</v>
       </c>
@@ -24025,7 +24046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B167" s="5" t="s">
         <v>169</v>
       </c>
@@ -24156,7 +24177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B168" s="5" t="s">
         <v>170</v>
       </c>
@@ -24287,7 +24308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B169" s="5" t="s">
         <v>171</v>
       </c>
@@ -24418,7 +24439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B170" s="5" t="s">
         <v>172</v>
       </c>
@@ -24549,7 +24570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B171" s="5" t="s">
         <v>173</v>
       </c>
@@ -24680,7 +24701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B172" s="5" t="s">
         <v>174</v>
       </c>
@@ -24811,7 +24832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A173" s="22" t="s">
         <v>318</v>
       </c>
@@ -24945,7 +24966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B174" s="5" t="s">
         <v>176</v>
       </c>
@@ -25076,7 +25097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B175" s="5" t="s">
         <v>177</v>
       </c>
@@ -25207,7 +25228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B176" s="5" t="s">
         <v>178</v>
       </c>
@@ -25338,7 +25359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B177" s="5" t="s">
         <v>179</v>
       </c>
@@ -25469,7 +25490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B178" s="5" t="s">
         <v>180</v>
       </c>
@@ -25600,7 +25621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B179" s="5" t="s">
         <v>181</v>
       </c>
@@ -25731,7 +25752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B180" s="5" t="s">
         <v>182</v>
       </c>
@@ -25862,9 +25883,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A181" s="22" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>183</v>
@@ -25996,7 +26017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B182" s="5" t="s">
         <v>184</v>
       </c>
@@ -26127,7 +26148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B183" s="5" t="s">
         <v>185</v>
       </c>
@@ -26258,7 +26279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B184" s="5" t="s">
         <v>186</v>
       </c>
@@ -26389,7 +26410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B185" s="5" t="s">
         <v>187</v>
       </c>
@@ -26520,7 +26541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B186" s="5" t="s">
         <v>188</v>
       </c>
@@ -26651,7 +26672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B187" s="5" t="s">
         <v>189</v>
       </c>
@@ -26782,7 +26803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B188" s="5" t="s">
         <v>190</v>
       </c>
@@ -26913,9 +26934,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A189" s="22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B189" s="5" t="s">
         <v>191</v>
@@ -27047,7 +27068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B190" s="5" t="s">
         <v>192</v>
       </c>
@@ -27178,7 +27199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B191" s="5" t="s">
         <v>193</v>
       </c>
@@ -27309,7 +27330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B192" s="5" t="s">
         <v>194</v>
       </c>
@@ -27440,7 +27461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B193" s="5" t="s">
         <v>195</v>
       </c>
@@ -27571,7 +27592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B194" s="5" t="s">
         <v>196</v>
       </c>
@@ -27702,7 +27723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B195" s="5" t="s">
         <v>197</v>
       </c>
@@ -27833,7 +27854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B196" s="5" t="s">
         <v>198</v>
       </c>
@@ -27964,9 +27985,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A197" s="22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>199</v>
@@ -28098,7 +28119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B198" s="5" t="s">
         <v>200</v>
       </c>
@@ -28229,7 +28250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B199" s="5" t="s">
         <v>201</v>
       </c>
@@ -28360,7 +28381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B200" s="5" t="s">
         <v>202</v>
       </c>
@@ -28491,7 +28512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B201" s="5" t="s">
         <v>203</v>
       </c>
@@ -28622,7 +28643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B202" s="5" t="s">
         <v>204</v>
       </c>
@@ -28753,7 +28774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B203" s="5" t="s">
         <v>205</v>
       </c>
@@ -28884,7 +28905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B204" s="5" t="s">
         <v>206</v>
       </c>
@@ -29015,9 +29036,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A205" s="22" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B205" s="5" t="s">
         <v>207</v>
@@ -29149,7 +29170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B206" s="5" t="s">
         <v>208</v>
       </c>
@@ -29280,7 +29301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B207" s="5" t="s">
         <v>209</v>
       </c>
@@ -29411,7 +29432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B208" s="5" t="s">
         <v>210</v>
       </c>
@@ -29542,7 +29563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B209" s="5" t="s">
         <v>211</v>
       </c>
@@ -29673,7 +29694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B210" s="5" t="s">
         <v>212</v>
       </c>
@@ -29804,7 +29825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B211" s="5" t="s">
         <v>213</v>
       </c>
@@ -29935,7 +29956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B212" s="5" t="s">
         <v>214</v>
       </c>
@@ -30066,9 +30087,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A213" s="22" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B213" s="5" t="s">
         <v>215</v>
@@ -30200,7 +30221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B214" s="5" t="s">
         <v>216</v>
       </c>
@@ -30331,7 +30352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B215" s="5" t="s">
         <v>217</v>
       </c>
@@ -30462,7 +30483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B216" s="5" t="s">
         <v>218</v>
       </c>
@@ -30593,7 +30614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B217" s="5" t="s">
         <v>219</v>
       </c>
@@ -30724,7 +30745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B218" s="5" t="s">
         <v>220</v>
       </c>
@@ -30855,7 +30876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B219" s="5" t="s">
         <v>221</v>
       </c>
@@ -30986,7 +31007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B220" s="5" t="s">
         <v>222</v>
       </c>
@@ -31117,9 +31138,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A221" s="22" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B221" s="5" t="s">
         <v>223</v>
@@ -31251,7 +31272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B222" s="5" t="s">
         <v>224</v>
       </c>
@@ -31382,7 +31403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B223" s="5" t="s">
         <v>225</v>
       </c>
@@ -31513,7 +31534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B224" s="5" t="s">
         <v>226</v>
       </c>
@@ -31644,7 +31665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B225" s="5" t="s">
         <v>227</v>
       </c>
@@ -31775,7 +31796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B226" s="5" t="s">
         <v>228</v>
       </c>
@@ -31906,7 +31927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B227" s="5" t="s">
         <v>229</v>
       </c>
@@ -32037,7 +32058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B228" s="5" t="s">
         <v>230</v>
       </c>
@@ -32168,9 +32189,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A229" s="22" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B229" s="5" t="s">
         <v>231</v>
@@ -32302,7 +32323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B230" s="5" t="s">
         <v>232</v>
       </c>
@@ -32433,7 +32454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B231" s="5" t="s">
         <v>233</v>
       </c>
@@ -32564,7 +32585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B232" s="5" t="s">
         <v>234</v>
       </c>
@@ -32695,7 +32716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B233" s="5" t="s">
         <v>235</v>
       </c>
@@ -32826,7 +32847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B234" s="5" t="s">
         <v>236</v>
       </c>
@@ -32957,7 +32978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B235" s="5" t="s">
         <v>237</v>
       </c>
@@ -33088,7 +33109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B236" s="5" t="s">
         <v>238</v>
       </c>
@@ -33219,7 +33240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A237" s="22" t="s">
         <v>301</v>
       </c>
@@ -33353,7 +33374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B238" s="5" t="s">
         <v>240</v>
       </c>
@@ -33484,7 +33505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B239" s="5" t="s">
         <v>241</v>
       </c>
@@ -33615,7 +33636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B240" s="5" t="s">
         <v>242</v>
       </c>
@@ -33746,7 +33767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B241" s="5" t="s">
         <v>243</v>
       </c>
@@ -33877,7 +33898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B242" s="5" t="s">
         <v>244</v>
       </c>
@@ -34008,7 +34029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B243" s="5" t="s">
         <v>245</v>
       </c>
@@ -34139,7 +34160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B244" s="5" t="s">
         <v>246</v>
       </c>
@@ -34270,7 +34291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A245" s="22" t="s">
         <v>264</v>
       </c>
@@ -34404,7 +34425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B246" s="5" t="s">
         <v>248</v>
       </c>
@@ -34535,7 +34556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B247" s="5" t="s">
         <v>249</v>
       </c>
@@ -34666,7 +34687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B248" s="5" t="s">
         <v>250</v>
       </c>
@@ -34797,7 +34818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B249" s="5" t="s">
         <v>251</v>
       </c>
@@ -34928,7 +34949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B250" s="5" t="s">
         <v>252</v>
       </c>
@@ -35059,7 +35080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B251" s="5" t="s">
         <v>253</v>
       </c>
@@ -35190,7 +35211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B252" s="5" t="s">
         <v>254</v>
       </c>
@@ -35321,7 +35342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A253" s="22" t="s">
         <v>316</v>
       </c>
@@ -35455,7 +35476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B254" s="5" t="s">
         <v>256</v>
       </c>
@@ -35586,7 +35607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B255" s="5" t="s">
         <v>257</v>
       </c>
@@ -35618,7 +35639,7 @@
         <v>0</v>
       </c>
       <c r="L255" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M255" s="8">
         <v>0</v>
@@ -35717,7 +35738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:44" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:44" x14ac:dyDescent="0.35">
       <c r="B256" s="5" t="s">
         <v>258</v>
       </c>
@@ -35848,7 +35869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="2:44" x14ac:dyDescent="0.4">
+    <row r="257" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B257" s="5" t="s">
         <v>259</v>
       </c>
@@ -35979,7 +36000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="2:44" x14ac:dyDescent="0.4">
+    <row r="258" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B258" s="5" t="s">
         <v>260</v>
       </c>
@@ -36110,7 +36131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="2:44" x14ac:dyDescent="0.4">
+    <row r="259" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B259" s="5" t="s">
         <v>261</v>
       </c>
@@ -36142,7 +36163,7 @@
         <v>0</v>
       </c>
       <c r="L259" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M259" s="8">
         <v>0</v>
@@ -36241,7 +36262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="2:44" x14ac:dyDescent="0.4">
+    <row r="260" spans="2:44" x14ac:dyDescent="0.35">
       <c r="B260" s="5" t="s">
         <v>262</v>
       </c>
@@ -36384,18 +36405,18 @@
     <mergeCell ref="U4:AB4"/>
     <mergeCell ref="AC4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:AJ30 I31:AJ31 I151:AJ151 E152:AJ158 I159:AJ159 E96:AJ150 E32:AJ93 E192:AR196 E160:AR172 E261:AJ1048576 AK237:AR246 E185:AR188 E221:AR223 E94:G94 I94:AJ95 E213:AJ213 X214:AJ214 E215:N215 P215:AJ215 I214:U214 E197:AJ198 I199:L199 P201:AJ202 R200 T200:AJ200 N199:AJ199 I216:AJ216 E217:AJ252 E203:AR203 I204:AR204 E202:H202 E205:AJ205 E206:G206 I206:N206 P206:AJ206 I207:L207 E210:AR212 E208:L209 M207:M209 O207:AJ209">
-    <cfRule type="cellIs" dxfId="58" priority="93" operator="equal">
+  <conditionalFormatting sqref="I31:AJ31 I151:AJ151 E152:AJ158 I159:AJ159 E96:AJ150 E32:AJ93 E192:AR196 E160:AR172 E261:AJ1048576 AK237:AR246 E185:AR188 E221:AR223 E94:G94 I94:AJ95 E213:AJ213 X214:AJ214 E215:N215 P215:AJ215 I214:U214 E197:AJ198 I199:L199 P201:AJ202 R200 T200:AJ200 N199:AJ199 I216:AJ216 E217:AJ252 E203:AR203 I204:AR204 E202:H202 E205:AJ205 E206:G206 I206:N206 P206:AJ206 I207:L207 E210:AR212 E208:L209 M207:M209 O207:AJ209 E5:AJ13 F14:G14 I14:AJ14 E15:AJ30 E253:AR254 E255:K255 M255:AR255 E256:AR259">
+    <cfRule type="cellIs" dxfId="61" priority="97" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:AJ4">
-    <cfRule type="cellIs" dxfId="57" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="94" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C1048576 C2:C3">
-    <cfRule type="colorScale" priority="95">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -36407,7 +36428,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D1048576 D2:D3">
-    <cfRule type="colorScale" priority="97">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -36419,286 +36440,301 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK5:AR148 AK152:AR156 AN149:AR151 AN157:AR159 AK220:AR252 AK261:AR1048576">
-    <cfRule type="cellIs" dxfId="56" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="93" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AR4">
-    <cfRule type="cellIs" dxfId="55" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK149:AM151">
-    <cfRule type="cellIs" dxfId="54" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="90" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK157:AM159">
-    <cfRule type="cellIs" dxfId="53" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="88" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E229:AJ231">
-    <cfRule type="cellIs" dxfId="52" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="85" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK229:AR231">
-    <cfRule type="cellIs" dxfId="51" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="84" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE238">
-    <cfRule type="cellIs" dxfId="50" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="83" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:H31">
-    <cfRule type="cellIs" dxfId="49" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="82" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E151:H151">
-    <cfRule type="cellIs" dxfId="48" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="81" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E159:H159">
+    <cfRule type="cellIs" dxfId="50" priority="80" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E95:G95">
+    <cfRule type="cellIs" dxfId="49" priority="79" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E243">
+    <cfRule type="cellIs" dxfId="48" priority="78" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K245">
     <cfRule type="cellIs" dxfId="47" priority="76" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95:G95">
-    <cfRule type="cellIs" dxfId="46" priority="75" operator="equal">
+  <conditionalFormatting sqref="E173:AJ180">
+    <cfRule type="cellIs" dxfId="46" priority="68" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E243">
-    <cfRule type="cellIs" dxfId="45" priority="74" operator="equal">
+  <conditionalFormatting sqref="AK173:AR180">
+    <cfRule type="cellIs" dxfId="45" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K245">
-    <cfRule type="cellIs" dxfId="44" priority="72" operator="equal">
+  <conditionalFormatting sqref="AK253:AR259">
+    <cfRule type="cellIs" dxfId="44" priority="65" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E173:AJ180">
+  <conditionalFormatting sqref="E253:AJ253 E254:AC254 AF254:AJ254 M259:AJ259">
     <cfRule type="cellIs" dxfId="43" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK173:AR180">
+  <conditionalFormatting sqref="AD258:AE258">
     <cfRule type="cellIs" dxfId="42" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E253:AR259">
+  <conditionalFormatting sqref="E260:L260">
     <cfRule type="cellIs" dxfId="41" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK253:AR259">
+  <conditionalFormatting sqref="M260:T260">
     <cfRule type="cellIs" dxfId="40" priority="61" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E253:AJ253 E254:AC254 AF254:AJ254 M259:AJ259">
+  <conditionalFormatting sqref="U260:AB260">
     <cfRule type="cellIs" dxfId="39" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD258:AE258">
+  <conditionalFormatting sqref="AC260:AJ260">
     <cfRule type="cellIs" dxfId="38" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E260:L260">
-    <cfRule type="cellIs" dxfId="37" priority="58" operator="equal">
+  <conditionalFormatting sqref="AK215:AR219">
+    <cfRule type="cellIs" dxfId="37" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M260:T260">
-    <cfRule type="cellIs" dxfId="36" priority="57" operator="equal">
+  <conditionalFormatting sqref="AK260:AR260">
+    <cfRule type="cellIs" dxfId="36" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U260:AB260">
-    <cfRule type="cellIs" dxfId="35" priority="56" operator="equal">
+  <conditionalFormatting sqref="E203:AR203 E200:O202">
+    <cfRule type="cellIs" dxfId="35" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC260:AJ260">
-    <cfRule type="cellIs" dxfId="34" priority="55" operator="equal">
+  <conditionalFormatting sqref="E200:O200">
+    <cfRule type="cellIs" dxfId="34" priority="51" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK215:AR219">
+  <conditionalFormatting sqref="E201:O202">
     <cfRule type="cellIs" dxfId="33" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK260:AR260">
-    <cfRule type="cellIs" dxfId="32" priority="54" operator="equal">
+  <conditionalFormatting sqref="E181:AJ182 I183:AJ183 E184:AJ184">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E203:AR203 E200:O202">
-    <cfRule type="cellIs" dxfId="31" priority="50" operator="equal">
+  <conditionalFormatting sqref="AK181:AR184">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E200:O200">
-    <cfRule type="cellIs" dxfId="30" priority="47" operator="equal">
+  <conditionalFormatting sqref="E183:H183">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E201:O202">
-    <cfRule type="cellIs" dxfId="29" priority="48" operator="equal">
+  <conditionalFormatting sqref="E189:AJ191">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E181:AJ182 I183:AJ183 E184:AJ184">
+  <conditionalFormatting sqref="AK189:AR191">
     <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK181:AR184">
+  <conditionalFormatting sqref="H94:H95">
     <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E183:H183">
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E189:AJ191">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK189:AR191">
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H94:H95">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AK213:AR214">
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V214:W214">
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O215">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E214:H214">
-    <cfRule type="cellIs" dxfId="19" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK197:AR199">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M199">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E199:H199">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E199:H199">
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK200:AR202">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P200">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q200">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S200">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E216:H216">
     <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P200">
+  <conditionalFormatting sqref="E204:H204">
     <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q200">
+  <conditionalFormatting sqref="E204:H204">
     <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S200">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+  <conditionalFormatting sqref="AK205:AR206">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E216:H216">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+  <conditionalFormatting sqref="H206">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E204:H204">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+  <conditionalFormatting sqref="O206">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E204:H204">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+  <conditionalFormatting sqref="E207:G207">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK205:AR206">
+  <conditionalFormatting sqref="H207">
     <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H206">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="AK207:AM208">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O206">
+  <conditionalFormatting sqref="AK209:AR209 AN207:AR208">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E207:G207">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+  <conditionalFormatting sqref="N207:N209">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H207">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK207:AM208">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="H14">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK209:AR209 AN207:AR208">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="L255">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N207:N209">
+  <conditionalFormatting sqref="L255">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>